<commit_message>
CIERRE 25 FEB 22
</commit_message>
<xml_diff>
--- a/01 DOCUEMENTOS/CENTRAL  ARCHIVO   2 0 2 2/CENTRAL #02  FEBRERO 2022/BALANCE    ZAVALETA   FEBRERO     2022 VALIDA.xlsx
+++ b/01 DOCUEMENTOS/CENTRAL  ARCHIVO   2 0 2 2/CENTRAL #02  FEBRERO 2022/BALANCE    ZAVALETA   FEBRERO     2022 VALIDA.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="3690" yWindow="0" windowWidth="16605" windowHeight="10920" firstSheet="7" activeTab="8"/>
+    <workbookView xWindow="3690" yWindow="0" windowWidth="16605" windowHeight="10920" firstSheet="6" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="OCTUBRE      2 0 2 1     " sheetId="1" r:id="rId1"/>
@@ -4445,6 +4445,39 @@
     <xf numFmtId="164" fontId="2" fillId="0" borderId="54" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="40" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="40" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="4" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="27" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -4517,45 +4550,60 @@
     <xf numFmtId="44" fontId="12" fillId="0" borderId="49" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="4" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="1" fontId="43" fillId="6" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="1" fontId="43" fillId="6" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="44" fontId="13" fillId="0" borderId="57" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="13" fillId="0" borderId="77" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="13" fillId="0" borderId="58" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="13" fillId="0" borderId="33" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="13" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="13" fillId="0" borderId="59" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="16" fillId="3" borderId="69" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="16" fillId="3" borderId="71" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="2" fillId="3" borderId="70" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="2" fillId="3" borderId="72" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="41" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="41" fillId="3" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="10" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="44" fontId="13" fillId="9" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -4582,54 +4630,6 @@
     </xf>
     <xf numFmtId="7" fontId="11" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="10" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="44" fontId="13" fillId="0" borderId="57" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="13" fillId="0" borderId="77" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="13" fillId="0" borderId="58" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="13" fillId="0" borderId="33" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="13" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="13" fillId="0" borderId="59" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="44" fontId="16" fillId="3" borderId="69" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="16" fillId="3" borderId="71" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="2" fillId="3" borderId="70" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="2" fillId="3" borderId="72" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="41" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="41" fillId="3" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="3" fillId="3" borderId="74" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -7329,23 +7329,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B1" s="465"/>
-      <c r="C1" s="467" t="s">
+      <c r="B1" s="441"/>
+      <c r="C1" s="443" t="s">
         <v>25</v>
       </c>
-      <c r="D1" s="468"/>
-      <c r="E1" s="468"/>
-      <c r="F1" s="468"/>
-      <c r="G1" s="468"/>
-      <c r="H1" s="468"/>
-      <c r="I1" s="468"/>
-      <c r="J1" s="468"/>
-      <c r="K1" s="468"/>
-      <c r="L1" s="468"/>
-      <c r="M1" s="468"/>
+      <c r="D1" s="444"/>
+      <c r="E1" s="444"/>
+      <c r="F1" s="444"/>
+      <c r="G1" s="444"/>
+      <c r="H1" s="444"/>
+      <c r="I1" s="444"/>
+      <c r="J1" s="444"/>
+      <c r="K1" s="444"/>
+      <c r="L1" s="444"/>
+      <c r="M1" s="444"/>
     </row>
     <row r="2" spans="1:19" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="466"/>
+      <c r="B2" s="442"/>
       <c r="C2" s="3"/>
       <c r="H2" s="5"/>
       <c r="I2" s="6"/>
@@ -7355,17 +7355,17 @@
       <c r="N2" s="9"/>
     </row>
     <row r="3" spans="1:19" ht="21.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="469" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="470"/>
+      <c r="B3" s="445" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="446"/>
       <c r="D3" s="10"/>
       <c r="E3" s="11"/>
       <c r="F3" s="11"/>
-      <c r="H3" s="471" t="s">
+      <c r="H3" s="447" t="s">
         <v>26</v>
       </c>
-      <c r="I3" s="471"/>
+      <c r="I3" s="447"/>
       <c r="K3" s="165"/>
       <c r="L3" s="13"/>
       <c r="M3" s="14"/>
@@ -7379,14 +7379,14 @@
         <v>0</v>
       </c>
       <c r="D4" s="18"/>
-      <c r="E4" s="472" t="s">
+      <c r="E4" s="448" t="s">
         <v>2</v>
       </c>
-      <c r="F4" s="473"/>
-      <c r="H4" s="474" t="s">
+      <c r="F4" s="449"/>
+      <c r="H4" s="450" t="s">
         <v>3</v>
       </c>
-      <c r="I4" s="475"/>
+      <c r="I4" s="451"/>
       <c r="J4" s="19"/>
       <c r="K4" s="166"/>
       <c r="L4" s="20"/>
@@ -7396,10 +7396,10 @@
       <c r="N4" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="P4" s="446" t="s">
+      <c r="P4" s="457" t="s">
         <v>6</v>
       </c>
-      <c r="Q4" s="447"/>
+      <c r="Q4" s="458"/>
     </row>
     <row r="5" spans="1:19" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="23" t="s">
@@ -8840,11 +8840,11 @@
       <c r="J39" s="60"/>
       <c r="K39" s="177"/>
       <c r="L39" s="61"/>
-      <c r="M39" s="448">
+      <c r="M39" s="459">
         <f>SUM(M5:M38)</f>
         <v>247061</v>
       </c>
-      <c r="N39" s="450">
+      <c r="N39" s="461">
         <f>SUM(N5:N38)</f>
         <v>172863</v>
       </c>
@@ -8870,8 +8870,8 @@
       <c r="J40" s="60"/>
       <c r="K40" s="41"/>
       <c r="L40" s="61"/>
-      <c r="M40" s="449"/>
-      <c r="N40" s="451"/>
+      <c r="M40" s="460"/>
+      <c r="N40" s="462"/>
       <c r="P40" s="34"/>
       <c r="Q40" s="9"/>
     </row>
@@ -9086,29 +9086,29 @@
       <c r="A52" s="98"/>
       <c r="B52" s="99"/>
       <c r="C52" s="1"/>
-      <c r="H52" s="452" t="s">
+      <c r="H52" s="463" t="s">
         <v>11</v>
       </c>
-      <c r="I52" s="453"/>
+      <c r="I52" s="464"/>
       <c r="J52" s="100"/>
-      <c r="K52" s="454">
+      <c r="K52" s="465">
         <f>I50+L50</f>
         <v>53873.49</v>
       </c>
-      <c r="L52" s="455"/>
-      <c r="M52" s="456">
+      <c r="L52" s="466"/>
+      <c r="M52" s="467">
         <f>N39+M39</f>
         <v>419924</v>
       </c>
-      <c r="N52" s="457"/>
+      <c r="N52" s="468"/>
       <c r="P52" s="34"/>
       <c r="Q52" s="9"/>
     </row>
     <row r="53" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="D53" s="458" t="s">
+      <c r="D53" s="469" t="s">
         <v>12</v>
       </c>
-      <c r="E53" s="458"/>
+      <c r="E53" s="469"/>
       <c r="F53" s="101">
         <f>F50-K52-C50</f>
         <v>471038.61</v>
@@ -9119,22 +9119,22 @@
       <c r="Q53" s="9"/>
     </row>
     <row r="54" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="D54" s="458" t="s">
+      <c r="D54" s="469" t="s">
         <v>95</v>
       </c>
-      <c r="E54" s="458"/>
+      <c r="E54" s="469"/>
       <c r="F54" s="96">
         <v>-549976.4</v>
       </c>
-      <c r="I54" s="459" t="s">
+      <c r="I54" s="470" t="s">
         <v>13</v>
       </c>
-      <c r="J54" s="460"/>
-      <c r="K54" s="461">
+      <c r="J54" s="471"/>
+      <c r="K54" s="472">
         <f>F56+F57+F58</f>
         <v>-24577.400000000023</v>
       </c>
-      <c r="L54" s="462"/>
+      <c r="L54" s="473"/>
       <c r="P54" s="34"/>
       <c r="Q54" s="9"/>
     </row>
@@ -9167,11 +9167,11 @@
         <v>15</v>
       </c>
       <c r="J56" s="109"/>
-      <c r="K56" s="463">
+      <c r="K56" s="474">
         <f>-C4</f>
         <v>0</v>
       </c>
-      <c r="L56" s="464"/>
+      <c r="L56" s="475"/>
     </row>
     <row r="57" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D57" s="110" t="s">
@@ -9188,22 +9188,22 @@
       <c r="C58" s="112">
         <v>44507</v>
       </c>
-      <c r="D58" s="441" t="s">
+      <c r="D58" s="452" t="s">
         <v>18</v>
       </c>
-      <c r="E58" s="442"/>
+      <c r="E58" s="453"/>
       <c r="F58" s="113">
         <v>567389.35</v>
       </c>
-      <c r="I58" s="443" t="s">
+      <c r="I58" s="454" t="s">
         <v>97</v>
       </c>
-      <c r="J58" s="444"/>
-      <c r="K58" s="445">
+      <c r="J58" s="455"/>
+      <c r="K58" s="456">
         <f>K54+K56</f>
         <v>-24577.400000000023</v>
       </c>
-      <c r="L58" s="445"/>
+      <c r="L58" s="456"/>
     </row>
     <row r="59" spans="1:17" ht="17.25" x14ac:dyDescent="0.3">
       <c r="C59" s="114"/>
@@ -9347,12 +9347,6 @@
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:M1"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="H3:I3"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="H4:I4"/>
     <mergeCell ref="D58:E58"/>
     <mergeCell ref="I58:J58"/>
     <mergeCell ref="K58:L58"/>
@@ -9367,6 +9361,12 @@
     <mergeCell ref="I54:J54"/>
     <mergeCell ref="K54:L54"/>
     <mergeCell ref="K56:L56"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:M1"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="H4:I4"/>
   </mergeCells>
   <pageMargins left="0.39370078740157483" right="0.15748031496062992" top="0.35433070866141736" bottom="0.31496062992125984" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup scale="75" orientation="landscape" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -14535,23 +14535,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:25" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B1" s="465"/>
-      <c r="C1" s="467" t="s">
+      <c r="B1" s="441"/>
+      <c r="C1" s="443" t="s">
         <v>208</v>
       </c>
-      <c r="D1" s="468"/>
-      <c r="E1" s="468"/>
-      <c r="F1" s="468"/>
-      <c r="G1" s="468"/>
-      <c r="H1" s="468"/>
-      <c r="I1" s="468"/>
-      <c r="J1" s="468"/>
-      <c r="K1" s="468"/>
-      <c r="L1" s="468"/>
-      <c r="M1" s="468"/>
+      <c r="D1" s="444"/>
+      <c r="E1" s="444"/>
+      <c r="F1" s="444"/>
+      <c r="G1" s="444"/>
+      <c r="H1" s="444"/>
+      <c r="I1" s="444"/>
+      <c r="J1" s="444"/>
+      <c r="K1" s="444"/>
+      <c r="L1" s="444"/>
+      <c r="M1" s="444"/>
     </row>
     <row r="2" spans="1:25" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="466"/>
+      <c r="B2" s="442"/>
       <c r="C2" s="3"/>
       <c r="H2" s="5"/>
       <c r="I2" s="6"/>
@@ -14561,21 +14561,21 @@
       <c r="N2" s="9"/>
     </row>
     <row r="3" spans="1:25" ht="21.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="469" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="470"/>
+      <c r="B3" s="445" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="446"/>
       <c r="D3" s="10"/>
       <c r="E3" s="11"/>
       <c r="F3" s="11"/>
-      <c r="H3" s="471" t="s">
+      <c r="H3" s="447" t="s">
         <v>26</v>
       </c>
-      <c r="I3" s="471"/>
+      <c r="I3" s="447"/>
       <c r="K3" s="165"/>
       <c r="L3" s="13"/>
       <c r="M3" s="14"/>
-      <c r="P3" s="495" t="s">
+      <c r="P3" s="484" t="s">
         <v>6</v>
       </c>
     </row>
@@ -14590,14 +14590,14 @@
       <c r="D4" s="18">
         <v>44507</v>
       </c>
-      <c r="E4" s="472" t="s">
+      <c r="E4" s="448" t="s">
         <v>2</v>
       </c>
-      <c r="F4" s="473"/>
-      <c r="H4" s="474" t="s">
+      <c r="F4" s="449"/>
+      <c r="H4" s="450" t="s">
         <v>3</v>
       </c>
-      <c r="I4" s="475"/>
+      <c r="I4" s="451"/>
       <c r="J4" s="19"/>
       <c r="K4" s="166"/>
       <c r="L4" s="20"/>
@@ -14607,14 +14607,14 @@
       <c r="N4" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="P4" s="496"/>
+      <c r="P4" s="485"/>
       <c r="Q4" s="286" t="s">
         <v>209</v>
       </c>
-      <c r="W4" s="478" t="s">
+      <c r="W4" s="494" t="s">
         <v>124</v>
       </c>
-      <c r="X4" s="478"/>
+      <c r="X4" s="494"/>
       <c r="Y4" s="227"/>
     </row>
     <row r="5" spans="1:25" ht="18" thickBot="1" x14ac:dyDescent="0.35">
@@ -14665,8 +14665,8 @@
         <f>20000+7936</f>
         <v>27936</v>
       </c>
-      <c r="W5" s="478"/>
-      <c r="X5" s="478"/>
+      <c r="W5" s="494"/>
+      <c r="X5" s="494"/>
       <c r="Y5" s="233"/>
     </row>
     <row r="6" spans="1:25" ht="18" thickBot="1" x14ac:dyDescent="0.35">
@@ -15437,7 +15437,7 @@
         <v>26370</v>
       </c>
       <c r="S19" s="147"/>
-      <c r="W19" s="482">
+      <c r="W19" s="498">
         <f>SUM(W6:W18)</f>
         <v>935136</v>
       </c>
@@ -15489,7 +15489,7 @@
         <v>16395.830000000002</v>
       </c>
       <c r="S20" s="147"/>
-      <c r="W20" s="483"/>
+      <c r="W20" s="499"/>
       <c r="X20" s="268"/>
       <c r="Y20" s="233"/>
     </row>
@@ -15538,8 +15538,8 @@
         <v>19188.82</v>
       </c>
       <c r="S21" s="147"/>
-      <c r="W21" s="484"/>
-      <c r="X21" s="484"/>
+      <c r="W21" s="500"/>
+      <c r="X21" s="500"/>
       <c r="Y21" s="233"/>
       <c r="Z21" s="128"/>
     </row>
@@ -15640,8 +15640,8 @@
         <v>45217.29</v>
       </c>
       <c r="S23" s="147"/>
-      <c r="W23" s="485"/>
-      <c r="X23" s="485"/>
+      <c r="W23" s="501"/>
+      <c r="X23" s="501"/>
       <c r="Y23" s="233"/>
       <c r="Z23" s="128"/>
     </row>
@@ -15695,8 +15695,8 @@
         <v>23159.17</v>
       </c>
       <c r="S24" s="147"/>
-      <c r="W24" s="485"/>
-      <c r="X24" s="485"/>
+      <c r="W24" s="501"/>
+      <c r="X24" s="501"/>
       <c r="Y24" s="233"/>
       <c r="Z24" s="128"/>
     </row>
@@ -15742,8 +15742,8 @@
       <c r="R25" s="285">
         <v>28952</v>
       </c>
-      <c r="W25" s="486"/>
-      <c r="X25" s="486"/>
+      <c r="W25" s="502"/>
+      <c r="X25" s="502"/>
       <c r="Y25" s="233"/>
       <c r="Z25" s="128"/>
     </row>
@@ -15794,8 +15794,8 @@
       <c r="R26" s="285">
         <v>21771.5</v>
       </c>
-      <c r="W26" s="486"/>
-      <c r="X26" s="486"/>
+      <c r="W26" s="502"/>
+      <c r="X26" s="502"/>
       <c r="Y26" s="233"/>
       <c r="Z26" s="128"/>
     </row>
@@ -15843,9 +15843,9 @@
       <c r="R27" s="285">
         <v>14637</v>
       </c>
-      <c r="W27" s="479"/>
-      <c r="X27" s="480"/>
-      <c r="Y27" s="481"/>
+      <c r="W27" s="495"/>
+      <c r="X27" s="496"/>
+      <c r="Y27" s="497"/>
       <c r="Z27" s="128"/>
     </row>
     <row r="28" spans="1:26" ht="18" thickBot="1" x14ac:dyDescent="0.35">
@@ -15895,9 +15895,9 @@
       <c r="R28" s="285">
         <v>0</v>
       </c>
-      <c r="W28" s="480"/>
-      <c r="X28" s="480"/>
-      <c r="Y28" s="481"/>
+      <c r="W28" s="496"/>
+      <c r="X28" s="496"/>
+      <c r="Y28" s="497"/>
       <c r="Z28" s="128"/>
     </row>
     <row r="29" spans="1:26" ht="18" thickBot="1" x14ac:dyDescent="0.35">
@@ -16232,11 +16232,11 @@
       <c r="L36" s="44">
         <v>5940</v>
       </c>
-      <c r="M36" s="497">
+      <c r="M36" s="486">
         <f>SUM(M5:M35)</f>
         <v>321168.83</v>
       </c>
-      <c r="N36" s="499">
+      <c r="N36" s="488">
         <f>SUM(N5:N35)</f>
         <v>467016</v>
       </c>
@@ -16244,7 +16244,7 @@
       <c r="P36" s="277">
         <v>0</v>
       </c>
-      <c r="Q36" s="501">
+      <c r="Q36" s="490">
         <f>SUM(Q5:Q35)</f>
         <v>-637069.14000000013</v>
       </c>
@@ -16279,13 +16279,13 @@
       <c r="L37" s="61">
         <v>7929.62</v>
       </c>
-      <c r="M37" s="498"/>
-      <c r="N37" s="500"/>
+      <c r="M37" s="487"/>
+      <c r="N37" s="489"/>
       <c r="O37" s="276"/>
       <c r="P37" s="277">
         <v>0</v>
       </c>
-      <c r="Q37" s="502"/>
+      <c r="Q37" s="491"/>
     </row>
     <row r="38" spans="1:18" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A38" s="23"/>
@@ -16575,26 +16575,26 @@
       <c r="A52" s="98"/>
       <c r="B52" s="99"/>
       <c r="C52" s="1"/>
-      <c r="H52" s="452" t="s">
+      <c r="H52" s="463" t="s">
         <v>11</v>
       </c>
-      <c r="I52" s="453"/>
+      <c r="I52" s="464"/>
       <c r="J52" s="100"/>
-      <c r="K52" s="454">
+      <c r="K52" s="465">
         <f>I50+L50</f>
         <v>71911.59</v>
       </c>
-      <c r="L52" s="487"/>
+      <c r="L52" s="492"/>
       <c r="M52" s="272"/>
       <c r="N52" s="272"/>
       <c r="P52" s="34"/>
       <c r="Q52" s="13"/>
     </row>
     <row r="53" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D53" s="458" t="s">
+      <c r="D53" s="469" t="s">
         <v>12</v>
       </c>
-      <c r="E53" s="458"/>
+      <c r="E53" s="469"/>
       <c r="F53" s="313">
         <f>F50-K52-C50</f>
         <v>-25952.549999999814</v>
@@ -16603,29 +16603,29 @@
       <c r="J53" s="103"/>
     </row>
     <row r="54" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="D54" s="488" t="s">
+      <c r="D54" s="493" t="s">
         <v>95</v>
       </c>
-      <c r="E54" s="488"/>
+      <c r="E54" s="493"/>
       <c r="F54" s="111">
         <v>-706888.38</v>
       </c>
-      <c r="I54" s="459" t="s">
+      <c r="I54" s="470" t="s">
         <v>13</v>
       </c>
-      <c r="J54" s="460"/>
-      <c r="K54" s="461">
+      <c r="J54" s="471"/>
+      <c r="K54" s="472">
         <f>F56+F57+F58</f>
         <v>1308778.3500000003</v>
       </c>
-      <c r="L54" s="461"/>
-      <c r="M54" s="489" t="s">
+      <c r="L54" s="472"/>
+      <c r="M54" s="478" t="s">
         <v>211</v>
       </c>
-      <c r="N54" s="490"/>
-      <c r="O54" s="490"/>
-      <c r="P54" s="490"/>
-      <c r="Q54" s="491"/>
+      <c r="N54" s="479"/>
+      <c r="O54" s="479"/>
+      <c r="P54" s="479"/>
+      <c r="Q54" s="480"/>
     </row>
     <row r="55" spans="1:17" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D55" s="314" t="s">
@@ -16639,11 +16639,11 @@
       <c r="J55" s="106"/>
       <c r="K55" s="178"/>
       <c r="L55" s="107"/>
-      <c r="M55" s="492"/>
-      <c r="N55" s="493"/>
-      <c r="O55" s="493"/>
-      <c r="P55" s="493"/>
-      <c r="Q55" s="494"/>
+      <c r="M55" s="481"/>
+      <c r="N55" s="482"/>
+      <c r="O55" s="482"/>
+      <c r="P55" s="482"/>
+      <c r="Q55" s="483"/>
     </row>
     <row r="56" spans="1:17" ht="19.5" thickTop="1" x14ac:dyDescent="0.3">
       <c r="C56" s="4" t="s">
@@ -16661,11 +16661,11 @@
         <v>15</v>
       </c>
       <c r="J56" s="109"/>
-      <c r="K56" s="463">
+      <c r="K56" s="474">
         <f>-C4</f>
         <v>-567389.35</v>
       </c>
-      <c r="L56" s="464"/>
+      <c r="L56" s="475"/>
     </row>
     <row r="57" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D57" s="110" t="s">
@@ -16682,22 +16682,22 @@
       <c r="C58" s="112">
         <v>44535</v>
       </c>
-      <c r="D58" s="441" t="s">
+      <c r="D58" s="452" t="s">
         <v>18</v>
       </c>
-      <c r="E58" s="442"/>
+      <c r="E58" s="453"/>
       <c r="F58" s="113">
         <v>2142307.62</v>
       </c>
-      <c r="I58" s="443" t="s">
+      <c r="I58" s="454" t="s">
         <v>198</v>
       </c>
-      <c r="J58" s="444"/>
-      <c r="K58" s="445">
+      <c r="J58" s="455"/>
+      <c r="K58" s="456">
         <f>K54+K56</f>
         <v>741389.00000000035</v>
       </c>
-      <c r="L58" s="445"/>
+      <c r="L58" s="456"/>
     </row>
     <row r="59" spans="1:17" ht="17.25" x14ac:dyDescent="0.3">
       <c r="C59" s="114"/>
@@ -16841,17 +16841,14 @@
     </row>
   </sheetData>
   <mergeCells count="29">
-    <mergeCell ref="M54:Q55"/>
-    <mergeCell ref="P3:P4"/>
-    <mergeCell ref="M36:M37"/>
-    <mergeCell ref="N36:N37"/>
-    <mergeCell ref="Q36:Q37"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:M1"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="H3:I3"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="H4:I4"/>
+    <mergeCell ref="W4:X5"/>
+    <mergeCell ref="W27:X28"/>
+    <mergeCell ref="Y27:Y28"/>
+    <mergeCell ref="W19:W20"/>
+    <mergeCell ref="W21:X21"/>
+    <mergeCell ref="W23:X24"/>
+    <mergeCell ref="W25:X25"/>
+    <mergeCell ref="W26:X26"/>
     <mergeCell ref="D58:E58"/>
     <mergeCell ref="I58:J58"/>
     <mergeCell ref="K58:L58"/>
@@ -16862,14 +16859,17 @@
     <mergeCell ref="I54:J54"/>
     <mergeCell ref="K54:L54"/>
     <mergeCell ref="K56:L56"/>
-    <mergeCell ref="W4:X5"/>
-    <mergeCell ref="W27:X28"/>
-    <mergeCell ref="Y27:Y28"/>
-    <mergeCell ref="W19:W20"/>
-    <mergeCell ref="W21:X21"/>
-    <mergeCell ref="W23:X24"/>
-    <mergeCell ref="W25:X25"/>
-    <mergeCell ref="W26:X26"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:M1"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="H4:I4"/>
+    <mergeCell ref="M54:Q55"/>
+    <mergeCell ref="P3:P4"/>
+    <mergeCell ref="M36:M37"/>
+    <mergeCell ref="N36:N37"/>
+    <mergeCell ref="Q36:Q37"/>
   </mergeCells>
   <pageMargins left="0.15748031496062992" right="0.15748031496062992" top="0.27559055118110237" bottom="0.27559055118110237" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup scale="68" orientation="landscape" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -19612,23 +19612,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:25" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B1" s="465"/>
-      <c r="C1" s="467" t="s">
+      <c r="B1" s="441"/>
+      <c r="C1" s="443" t="s">
         <v>208</v>
       </c>
-      <c r="D1" s="468"/>
-      <c r="E1" s="468"/>
-      <c r="F1" s="468"/>
-      <c r="G1" s="468"/>
-      <c r="H1" s="468"/>
-      <c r="I1" s="468"/>
-      <c r="J1" s="468"/>
-      <c r="K1" s="468"/>
-      <c r="L1" s="468"/>
-      <c r="M1" s="468"/>
+      <c r="D1" s="444"/>
+      <c r="E1" s="444"/>
+      <c r="F1" s="444"/>
+      <c r="G1" s="444"/>
+      <c r="H1" s="444"/>
+      <c r="I1" s="444"/>
+      <c r="J1" s="444"/>
+      <c r="K1" s="444"/>
+      <c r="L1" s="444"/>
+      <c r="M1" s="444"/>
     </row>
     <row r="2" spans="1:25" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="466"/>
+      <c r="B2" s="442"/>
       <c r="C2" s="3"/>
       <c r="H2" s="5"/>
       <c r="I2" s="6"/>
@@ -19638,21 +19638,21 @@
       <c r="N2" s="9"/>
     </row>
     <row r="3" spans="1:25" ht="21.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="469" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="470"/>
+      <c r="B3" s="445" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="446"/>
       <c r="D3" s="10"/>
       <c r="E3" s="11"/>
       <c r="F3" s="11"/>
-      <c r="H3" s="471" t="s">
+      <c r="H3" s="447" t="s">
         <v>26</v>
       </c>
-      <c r="I3" s="471"/>
+      <c r="I3" s="447"/>
       <c r="K3" s="165"/>
       <c r="L3" s="13"/>
       <c r="M3" s="14"/>
-      <c r="P3" s="495" t="s">
+      <c r="P3" s="484" t="s">
         <v>6</v>
       </c>
       <c r="R3" s="505" t="s">
@@ -19670,14 +19670,14 @@
       <c r="D4" s="18">
         <v>44507</v>
       </c>
-      <c r="E4" s="472" t="s">
+      <c r="E4" s="448" t="s">
         <v>2</v>
       </c>
-      <c r="F4" s="473"/>
-      <c r="H4" s="474" t="s">
+      <c r="F4" s="449"/>
+      <c r="H4" s="450" t="s">
         <v>3</v>
       </c>
-      <c r="I4" s="475"/>
+      <c r="I4" s="451"/>
       <c r="J4" s="19"/>
       <c r="K4" s="166"/>
       <c r="L4" s="20"/>
@@ -19687,15 +19687,15 @@
       <c r="N4" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="P4" s="496"/>
+      <c r="P4" s="485"/>
       <c r="Q4" s="323" t="s">
         <v>217</v>
       </c>
       <c r="R4" s="506"/>
-      <c r="W4" s="478" t="s">
+      <c r="W4" s="494" t="s">
         <v>124</v>
       </c>
-      <c r="X4" s="478"/>
+      <c r="X4" s="494"/>
       <c r="Y4" s="227"/>
     </row>
     <row r="5" spans="1:25" ht="18" thickBot="1" x14ac:dyDescent="0.35">
@@ -19756,8 +19756,8 @@
       <c r="S5" s="325" t="s">
         <v>213</v>
       </c>
-      <c r="W5" s="478"/>
-      <c r="X5" s="478"/>
+      <c r="W5" s="494"/>
+      <c r="X5" s="494"/>
       <c r="Y5" s="233"/>
     </row>
     <row r="6" spans="1:25" ht="18" thickBot="1" x14ac:dyDescent="0.35">
@@ -20514,7 +20514,7 @@
         <v>0</v>
       </c>
       <c r="S19" s="147"/>
-      <c r="W19" s="482">
+      <c r="W19" s="498">
         <f>SUM(W6:W18)</f>
         <v>0</v>
       </c>
@@ -20566,7 +20566,7 @@
         <v>0</v>
       </c>
       <c r="S20" s="147"/>
-      <c r="W20" s="483"/>
+      <c r="W20" s="499"/>
       <c r="X20" s="268"/>
       <c r="Y20" s="233"/>
     </row>
@@ -20615,8 +20615,8 @@
         <v>0</v>
       </c>
       <c r="S21" s="147"/>
-      <c r="W21" s="484"/>
-      <c r="X21" s="484"/>
+      <c r="W21" s="500"/>
+      <c r="X21" s="500"/>
       <c r="Y21" s="233"/>
       <c r="Z21" s="128"/>
     </row>
@@ -20717,8 +20717,8 @@
         <v>0</v>
       </c>
       <c r="S23" s="147"/>
-      <c r="W23" s="485"/>
-      <c r="X23" s="485"/>
+      <c r="W23" s="501"/>
+      <c r="X23" s="501"/>
       <c r="Y23" s="233"/>
       <c r="Z23" s="128"/>
     </row>
@@ -20769,8 +20769,8 @@
         <v>0</v>
       </c>
       <c r="S24" s="147"/>
-      <c r="W24" s="485"/>
-      <c r="X24" s="485"/>
+      <c r="W24" s="501"/>
+      <c r="X24" s="501"/>
       <c r="Y24" s="233"/>
       <c r="Z24" s="128"/>
     </row>
@@ -20816,8 +20816,8 @@
       <c r="R25" s="320">
         <v>0</v>
       </c>
-      <c r="W25" s="486"/>
-      <c r="X25" s="486"/>
+      <c r="W25" s="502"/>
+      <c r="X25" s="502"/>
       <c r="Y25" s="233"/>
       <c r="Z25" s="128"/>
     </row>
@@ -20865,8 +20865,8 @@
       <c r="R26" s="320">
         <v>0</v>
       </c>
-      <c r="W26" s="486"/>
-      <c r="X26" s="486"/>
+      <c r="W26" s="502"/>
+      <c r="X26" s="502"/>
       <c r="Y26" s="233"/>
       <c r="Z26" s="128"/>
     </row>
@@ -20926,9 +20926,9 @@
       <c r="V27" t="s">
         <v>240</v>
       </c>
-      <c r="W27" s="479"/>
-      <c r="X27" s="480"/>
-      <c r="Y27" s="481"/>
+      <c r="W27" s="495"/>
+      <c r="X27" s="496"/>
+      <c r="Y27" s="497"/>
       <c r="Z27" s="128"/>
     </row>
     <row r="28" spans="1:26" ht="18" thickBot="1" x14ac:dyDescent="0.35">
@@ -20982,9 +20982,9 @@
       <c r="V28" t="s">
         <v>240</v>
       </c>
-      <c r="W28" s="480"/>
-      <c r="X28" s="480"/>
-      <c r="Y28" s="481"/>
+      <c r="W28" s="496"/>
+      <c r="X28" s="496"/>
+      <c r="Y28" s="497"/>
       <c r="Z28" s="128"/>
     </row>
     <row r="29" spans="1:26" ht="18" thickBot="1" x14ac:dyDescent="0.35">
@@ -21300,11 +21300,11 @@
       <c r="J36" s="266"/>
       <c r="K36" s="250"/>
       <c r="L36" s="44"/>
-      <c r="M36" s="497">
+      <c r="M36" s="486">
         <f>SUM(M5:M35)</f>
         <v>1077791.3</v>
       </c>
-      <c r="N36" s="499">
+      <c r="N36" s="488">
         <f>SUM(N5:N35)</f>
         <v>936398</v>
       </c>
@@ -21312,7 +21312,7 @@
       <c r="P36" s="277">
         <v>0</v>
       </c>
-      <c r="Q36" s="501">
+      <c r="Q36" s="490">
         <f>SUM(Q5:Q35)</f>
         <v>-14262.940000000002</v>
       </c>
@@ -21331,13 +21331,13 @@
       <c r="J37" s="60"/>
       <c r="K37" s="41"/>
       <c r="L37" s="61"/>
-      <c r="M37" s="498"/>
-      <c r="N37" s="500"/>
+      <c r="M37" s="487"/>
+      <c r="N37" s="489"/>
       <c r="O37" s="276"/>
       <c r="P37" s="277">
         <v>0</v>
       </c>
-      <c r="Q37" s="502"/>
+      <c r="Q37" s="491"/>
     </row>
     <row r="38" spans="1:18" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A38" s="23"/>
@@ -21611,26 +21611,26 @@
       <c r="A52" s="98"/>
       <c r="B52" s="99"/>
       <c r="C52" s="1"/>
-      <c r="H52" s="452" t="s">
+      <c r="H52" s="463" t="s">
         <v>11</v>
       </c>
-      <c r="I52" s="453"/>
+      <c r="I52" s="464"/>
       <c r="J52" s="100"/>
-      <c r="K52" s="454">
+      <c r="K52" s="465">
         <f>I50+L50</f>
         <v>90750.75</v>
       </c>
-      <c r="L52" s="487"/>
+      <c r="L52" s="492"/>
       <c r="M52" s="272"/>
       <c r="N52" s="272"/>
       <c r="P52" s="34"/>
       <c r="Q52" s="13"/>
     </row>
     <row r="53" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D53" s="458" t="s">
+      <c r="D53" s="469" t="s">
         <v>12</v>
       </c>
-      <c r="E53" s="458"/>
+      <c r="E53" s="469"/>
       <c r="F53" s="313">
         <f>F50-K52-C50</f>
         <v>1739855.03</v>
@@ -21639,29 +21639,29 @@
       <c r="J53" s="103"/>
     </row>
     <row r="54" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="D54" s="488" t="s">
+      <c r="D54" s="493" t="s">
         <v>95</v>
       </c>
-      <c r="E54" s="488"/>
+      <c r="E54" s="493"/>
       <c r="F54" s="111">
         <v>-1567070.66</v>
       </c>
-      <c r="I54" s="459" t="s">
+      <c r="I54" s="470" t="s">
         <v>13</v>
       </c>
-      <c r="J54" s="460"/>
-      <c r="K54" s="461">
+      <c r="J54" s="471"/>
+      <c r="K54" s="472">
         <f>F56+F57+F58</f>
         <v>703192.8600000001</v>
       </c>
-      <c r="L54" s="461"/>
-      <c r="M54" s="489" t="s">
+      <c r="L54" s="472"/>
+      <c r="M54" s="478" t="s">
         <v>211</v>
       </c>
-      <c r="N54" s="490"/>
-      <c r="O54" s="490"/>
-      <c r="P54" s="490"/>
-      <c r="Q54" s="491"/>
+      <c r="N54" s="479"/>
+      <c r="O54" s="479"/>
+      <c r="P54" s="479"/>
+      <c r="Q54" s="480"/>
     </row>
     <row r="55" spans="1:17" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D55" s="314" t="s">
@@ -21675,11 +21675,11 @@
       <c r="J55" s="106"/>
       <c r="K55" s="178"/>
       <c r="L55" s="107"/>
-      <c r="M55" s="492"/>
-      <c r="N55" s="493"/>
-      <c r="O55" s="493"/>
-      <c r="P55" s="493"/>
-      <c r="Q55" s="494"/>
+      <c r="M55" s="481"/>
+      <c r="N55" s="482"/>
+      <c r="O55" s="482"/>
+      <c r="P55" s="482"/>
+      <c r="Q55" s="483"/>
     </row>
     <row r="56" spans="1:17" ht="19.5" thickTop="1" x14ac:dyDescent="0.3">
       <c r="C56" s="4" t="s">
@@ -21697,11 +21697,11 @@
         <v>15</v>
       </c>
       <c r="J56" s="109"/>
-      <c r="K56" s="463">
+      <c r="K56" s="474">
         <f>-C4</f>
         <v>-567389.35</v>
       </c>
-      <c r="L56" s="464"/>
+      <c r="L56" s="475"/>
     </row>
     <row r="57" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D57" s="110" t="s">
@@ -21718,22 +21718,22 @@
       <c r="C58" s="112">
         <v>44563</v>
       </c>
-      <c r="D58" s="441" t="s">
+      <c r="D58" s="452" t="s">
         <v>18</v>
       </c>
-      <c r="E58" s="442"/>
+      <c r="E58" s="453"/>
       <c r="F58" s="113">
         <v>754143.23</v>
       </c>
-      <c r="I58" s="443" t="s">
+      <c r="I58" s="454" t="s">
         <v>198</v>
       </c>
-      <c r="J58" s="444"/>
-      <c r="K58" s="445">
+      <c r="J58" s="455"/>
+      <c r="K58" s="456">
         <f>K54+K56</f>
         <v>135803.51000000013</v>
       </c>
-      <c r="L58" s="445"/>
+      <c r="L58" s="456"/>
     </row>
     <row r="59" spans="1:17" ht="17.25" x14ac:dyDescent="0.3">
       <c r="C59" s="114"/>
@@ -21877,13 +21877,20 @@
     </row>
   </sheetData>
   <mergeCells count="30">
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:M1"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="H3:I3"/>
-    <mergeCell ref="P3:P4"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="H4:I4"/>
+    <mergeCell ref="D58:E58"/>
+    <mergeCell ref="I58:J58"/>
+    <mergeCell ref="K58:L58"/>
+    <mergeCell ref="D53:E53"/>
+    <mergeCell ref="D54:E54"/>
+    <mergeCell ref="I54:J54"/>
+    <mergeCell ref="K54:L54"/>
+    <mergeCell ref="M54:Q55"/>
+    <mergeCell ref="K56:L56"/>
+    <mergeCell ref="W27:X28"/>
+    <mergeCell ref="Y27:Y28"/>
+    <mergeCell ref="M36:M37"/>
+    <mergeCell ref="N36:N37"/>
+    <mergeCell ref="Q36:Q37"/>
     <mergeCell ref="H52:I52"/>
     <mergeCell ref="K52:L52"/>
     <mergeCell ref="W4:X5"/>
@@ -21893,20 +21900,13 @@
     <mergeCell ref="W25:X25"/>
     <mergeCell ref="W26:X26"/>
     <mergeCell ref="R3:R4"/>
-    <mergeCell ref="M54:Q55"/>
-    <mergeCell ref="K56:L56"/>
-    <mergeCell ref="W27:X28"/>
-    <mergeCell ref="Y27:Y28"/>
-    <mergeCell ref="M36:M37"/>
-    <mergeCell ref="N36:N37"/>
-    <mergeCell ref="Q36:Q37"/>
-    <mergeCell ref="D58:E58"/>
-    <mergeCell ref="I58:J58"/>
-    <mergeCell ref="K58:L58"/>
-    <mergeCell ref="D53:E53"/>
-    <mergeCell ref="D54:E54"/>
-    <mergeCell ref="I54:J54"/>
-    <mergeCell ref="K54:L54"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:M1"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="P3:P4"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="H4:I4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -24601,7 +24601,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:25" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B1" s="465"/>
+      <c r="B1" s="441"/>
       <c r="C1" s="507" t="s">
         <v>323</v>
       </c>
@@ -24617,7 +24617,7 @@
       <c r="M1" s="508"/>
     </row>
     <row r="2" spans="1:25" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="466"/>
+      <c r="B2" s="442"/>
       <c r="C2" s="3"/>
       <c r="H2" s="5"/>
       <c r="I2" s="6"/>
@@ -24627,21 +24627,21 @@
       <c r="N2" s="9"/>
     </row>
     <row r="3" spans="1:25" ht="21.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="469" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="470"/>
+      <c r="B3" s="445" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="446"/>
       <c r="D3" s="10"/>
       <c r="E3" s="11"/>
       <c r="F3" s="11"/>
-      <c r="H3" s="471" t="s">
+      <c r="H3" s="447" t="s">
         <v>26</v>
       </c>
-      <c r="I3" s="471"/>
+      <c r="I3" s="447"/>
       <c r="K3" s="165"/>
       <c r="L3" s="13"/>
       <c r="M3" s="14"/>
-      <c r="P3" s="495" t="s">
+      <c r="P3" s="484" t="s">
         <v>6</v>
       </c>
       <c r="R3" s="505" t="s">
@@ -24659,14 +24659,14 @@
       <c r="D4" s="18">
         <v>44563</v>
       </c>
-      <c r="E4" s="472" t="s">
+      <c r="E4" s="448" t="s">
         <v>2</v>
       </c>
-      <c r="F4" s="473"/>
-      <c r="H4" s="474" t="s">
+      <c r="F4" s="449"/>
+      <c r="H4" s="450" t="s">
         <v>3</v>
       </c>
-      <c r="I4" s="475"/>
+      <c r="I4" s="451"/>
       <c r="J4" s="19"/>
       <c r="K4" s="166"/>
       <c r="L4" s="20"/>
@@ -24676,15 +24676,15 @@
       <c r="N4" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="P4" s="496"/>
+      <c r="P4" s="485"/>
       <c r="Q4" s="323" t="s">
         <v>217</v>
       </c>
       <c r="R4" s="506"/>
-      <c r="W4" s="478" t="s">
+      <c r="W4" s="494" t="s">
         <v>124</v>
       </c>
-      <c r="X4" s="478"/>
+      <c r="X4" s="494"/>
       <c r="Y4" s="227"/>
     </row>
     <row r="5" spans="1:25" ht="18" thickBot="1" x14ac:dyDescent="0.35">
@@ -24735,8 +24735,8 @@
         <v>0</v>
       </c>
       <c r="S5" s="325"/>
-      <c r="W5" s="478"/>
-      <c r="X5" s="478"/>
+      <c r="W5" s="494"/>
+      <c r="X5" s="494"/>
       <c r="Y5" s="233"/>
     </row>
     <row r="6" spans="1:25" ht="18" thickBot="1" x14ac:dyDescent="0.35">
@@ -25500,7 +25500,7 @@
         <v>0</v>
       </c>
       <c r="S19" s="147"/>
-      <c r="W19" s="482">
+      <c r="W19" s="498">
         <f>SUM(W6:W18)</f>
         <v>0</v>
       </c>
@@ -25553,7 +25553,7 @@
         <v>0</v>
       </c>
       <c r="S20" s="147"/>
-      <c r="W20" s="483"/>
+      <c r="W20" s="499"/>
       <c r="X20" s="268"/>
       <c r="Y20" s="233"/>
     </row>
@@ -25602,8 +25602,8 @@
         <v>377273.87</v>
       </c>
       <c r="S21" s="147"/>
-      <c r="W21" s="484"/>
-      <c r="X21" s="484"/>
+      <c r="W21" s="500"/>
+      <c r="X21" s="500"/>
       <c r="Y21" s="233"/>
       <c r="Z21" s="128"/>
     </row>
@@ -25703,8 +25703,8 @@
         <v>0</v>
       </c>
       <c r="S23" s="147"/>
-      <c r="W23" s="485"/>
-      <c r="X23" s="485"/>
+      <c r="W23" s="501"/>
+      <c r="X23" s="501"/>
       <c r="Y23" s="233"/>
       <c r="Z23" s="128"/>
     </row>
@@ -25759,8 +25759,8 @@
         <v>0</v>
       </c>
       <c r="S24" s="147"/>
-      <c r="W24" s="485"/>
-      <c r="X24" s="485"/>
+      <c r="W24" s="501"/>
+      <c r="X24" s="501"/>
       <c r="Y24" s="233"/>
       <c r="Z24" s="128"/>
     </row>
@@ -25805,8 +25805,8 @@
       <c r="R25" s="320">
         <v>0</v>
       </c>
-      <c r="W25" s="486"/>
-      <c r="X25" s="486"/>
+      <c r="W25" s="502"/>
+      <c r="X25" s="502"/>
       <c r="Y25" s="233"/>
       <c r="Z25" s="128"/>
     </row>
@@ -25854,8 +25854,8 @@
       <c r="R26" s="320">
         <v>0</v>
       </c>
-      <c r="W26" s="486"/>
-      <c r="X26" s="486"/>
+      <c r="W26" s="502"/>
+      <c r="X26" s="502"/>
       <c r="Y26" s="233"/>
       <c r="Z26" s="128"/>
     </row>
@@ -25909,9 +25909,9 @@
       <c r="V27" t="s">
         <v>240</v>
       </c>
-      <c r="W27" s="479"/>
-      <c r="X27" s="480"/>
-      <c r="Y27" s="481"/>
+      <c r="W27" s="495"/>
+      <c r="X27" s="496"/>
+      <c r="Y27" s="497"/>
       <c r="Z27" s="128"/>
     </row>
     <row r="28" spans="1:26" ht="18" thickBot="1" x14ac:dyDescent="0.35">
@@ -25965,9 +25965,9 @@
       <c r="V28" t="s">
         <v>240</v>
       </c>
-      <c r="W28" s="480"/>
-      <c r="X28" s="480"/>
-      <c r="Y28" s="481"/>
+      <c r="W28" s="496"/>
+      <c r="X28" s="496"/>
+      <c r="Y28" s="497"/>
       <c r="Z28" s="128"/>
     </row>
     <row r="29" spans="1:26" ht="18" thickBot="1" x14ac:dyDescent="0.35">
@@ -26272,11 +26272,11 @@
       <c r="L36" s="44">
         <v>13275.84</v>
       </c>
-      <c r="M36" s="497">
+      <c r="M36" s="486">
         <f>SUM(M5:M35)</f>
         <v>1818445.73</v>
       </c>
-      <c r="N36" s="499">
+      <c r="N36" s="488">
         <f>SUM(N5:N35)</f>
         <v>739014</v>
       </c>
@@ -26284,7 +26284,7 @@
       <c r="P36" s="277">
         <v>0</v>
       </c>
-      <c r="Q36" s="501">
+      <c r="Q36" s="490">
         <f>SUM(Q5:Q35)</f>
         <v>-7.2800000000133878</v>
       </c>
@@ -26309,13 +26309,13 @@
       <c r="L37" s="61">
         <v>15060.32</v>
       </c>
-      <c r="M37" s="498"/>
-      <c r="N37" s="500"/>
+      <c r="M37" s="487"/>
+      <c r="N37" s="489"/>
       <c r="O37" s="276"/>
       <c r="P37" s="277">
         <v>0</v>
       </c>
-      <c r="Q37" s="502"/>
+      <c r="Q37" s="491"/>
       <c r="R37" s="227" t="s">
         <v>7</v>
       </c>
@@ -26602,26 +26602,26 @@
       <c r="A52" s="98"/>
       <c r="B52" s="99"/>
       <c r="C52" s="1"/>
-      <c r="H52" s="452" t="s">
+      <c r="H52" s="463" t="s">
         <v>11</v>
       </c>
-      <c r="I52" s="453"/>
+      <c r="I52" s="464"/>
       <c r="J52" s="100"/>
-      <c r="K52" s="454">
+      <c r="K52" s="465">
         <f>I50+L50</f>
         <v>144994.20000000001</v>
       </c>
-      <c r="L52" s="487"/>
+      <c r="L52" s="492"/>
       <c r="M52" s="272"/>
       <c r="N52" s="272"/>
       <c r="P52" s="34"/>
       <c r="Q52" s="13"/>
     </row>
     <row r="53" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="D53" s="458" t="s">
+      <c r="D53" s="469" t="s">
         <v>12</v>
       </c>
-      <c r="E53" s="458"/>
+      <c r="E53" s="469"/>
       <c r="F53" s="313">
         <f>F50-K52-C50</f>
         <v>2135426.1199999996</v>
@@ -26630,22 +26630,22 @@
       <c r="J53" s="103"/>
     </row>
     <row r="54" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="D54" s="488" t="s">
+      <c r="D54" s="493" t="s">
         <v>95</v>
       </c>
-      <c r="E54" s="488"/>
+      <c r="E54" s="493"/>
       <c r="F54" s="111">
         <v>-1448401.2</v>
       </c>
-      <c r="I54" s="459" t="s">
+      <c r="I54" s="470" t="s">
         <v>13</v>
       </c>
-      <c r="J54" s="460"/>
-      <c r="K54" s="461">
+      <c r="J54" s="471"/>
+      <c r="K54" s="472">
         <f>F56+F57+F58</f>
         <v>1082916.0699999996</v>
       </c>
-      <c r="L54" s="461"/>
+      <c r="L54" s="472"/>
       <c r="M54" s="423"/>
       <c r="N54" s="423"/>
       <c r="O54" s="423"/>
@@ -26686,11 +26686,11 @@
         <v>15</v>
       </c>
       <c r="J56" s="109"/>
-      <c r="K56" s="463">
+      <c r="K56" s="474">
         <f>-C4</f>
         <v>-754143.23</v>
       </c>
-      <c r="L56" s="464"/>
+      <c r="L56" s="475"/>
     </row>
     <row r="57" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D57" s="110" t="s">
@@ -26707,22 +26707,22 @@
       <c r="C58" s="112">
         <v>44591</v>
       </c>
-      <c r="D58" s="441" t="s">
+      <c r="D58" s="452" t="s">
         <v>18</v>
       </c>
-      <c r="E58" s="442"/>
+      <c r="E58" s="453"/>
       <c r="F58" s="113">
         <v>1149740.4099999999</v>
       </c>
-      <c r="I58" s="443" t="s">
+      <c r="I58" s="454" t="s">
         <v>198</v>
       </c>
-      <c r="J58" s="444"/>
-      <c r="K58" s="445">
+      <c r="J58" s="455"/>
+      <c r="K58" s="456">
         <f>K54+K56</f>
         <v>328772.83999999962</v>
       </c>
-      <c r="L58" s="445"/>
+      <c r="L58" s="456"/>
     </row>
     <row r="59" spans="1:17" ht="17.25" x14ac:dyDescent="0.3">
       <c r="C59" s="114"/>
@@ -26866,6 +26866,20 @@
     </row>
   </sheetData>
   <mergeCells count="29">
+    <mergeCell ref="Y27:Y28"/>
+    <mergeCell ref="M36:M37"/>
+    <mergeCell ref="N36:N37"/>
+    <mergeCell ref="Q36:Q37"/>
+    <mergeCell ref="D58:E58"/>
+    <mergeCell ref="I58:J58"/>
+    <mergeCell ref="K58:L58"/>
+    <mergeCell ref="D53:E53"/>
+    <mergeCell ref="D54:E54"/>
+    <mergeCell ref="I54:J54"/>
+    <mergeCell ref="K54:L54"/>
+    <mergeCell ref="K56:L56"/>
+    <mergeCell ref="H52:I52"/>
+    <mergeCell ref="K52:L52"/>
     <mergeCell ref="W26:X26"/>
     <mergeCell ref="R3:R4"/>
     <mergeCell ref="W27:X28"/>
@@ -26881,20 +26895,6 @@
     <mergeCell ref="W21:X21"/>
     <mergeCell ref="W23:X24"/>
     <mergeCell ref="W25:X25"/>
-    <mergeCell ref="Y27:Y28"/>
-    <mergeCell ref="M36:M37"/>
-    <mergeCell ref="N36:N37"/>
-    <mergeCell ref="Q36:Q37"/>
-    <mergeCell ref="D58:E58"/>
-    <mergeCell ref="I58:J58"/>
-    <mergeCell ref="K58:L58"/>
-    <mergeCell ref="D53:E53"/>
-    <mergeCell ref="D54:E54"/>
-    <mergeCell ref="I54:J54"/>
-    <mergeCell ref="K54:L54"/>
-    <mergeCell ref="K56:L56"/>
-    <mergeCell ref="H52:I52"/>
-    <mergeCell ref="K52:L52"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -26910,8 +26910,8 @@
   </sheetPr>
   <dimension ref="A1:N115"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="A25" sqref="A1:XFD1048576"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D49" sqref="D49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -29649,8 +29649,8 @@
   </sheetPr>
   <dimension ref="A1:Z80"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="Q18" sqref="Q18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J19" sqref="J19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -29679,7 +29679,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:25" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B1" s="465"/>
+      <c r="B1" s="441"/>
       <c r="C1" s="507" t="s">
         <v>323</v>
       </c>
@@ -29695,7 +29695,7 @@
       <c r="M1" s="508"/>
     </row>
     <row r="2" spans="1:25" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="466"/>
+      <c r="B2" s="442"/>
       <c r="C2" s="3"/>
       <c r="H2" s="5"/>
       <c r="I2" s="6"/>
@@ -29705,21 +29705,21 @@
       <c r="N2" s="9"/>
     </row>
     <row r="3" spans="1:25" ht="21.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="469" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="470"/>
+      <c r="B3" s="445" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="446"/>
       <c r="D3" s="10"/>
       <c r="E3" s="11"/>
       <c r="F3" s="11"/>
-      <c r="H3" s="471" t="s">
+      <c r="H3" s="447" t="s">
         <v>26</v>
       </c>
-      <c r="I3" s="471"/>
+      <c r="I3" s="447"/>
       <c r="K3" s="165"/>
       <c r="L3" s="13"/>
       <c r="M3" s="14"/>
-      <c r="P3" s="495" t="s">
+      <c r="P3" s="484" t="s">
         <v>6</v>
       </c>
       <c r="R3" s="505" t="s">
@@ -29737,14 +29737,14 @@
       <c r="D4" s="18">
         <v>44591</v>
       </c>
-      <c r="E4" s="472" t="s">
+      <c r="E4" s="448" t="s">
         <v>2</v>
       </c>
-      <c r="F4" s="473"/>
-      <c r="H4" s="474" t="s">
+      <c r="F4" s="449"/>
+      <c r="H4" s="450" t="s">
         <v>3</v>
       </c>
-      <c r="I4" s="475"/>
+      <c r="I4" s="451"/>
       <c r="J4" s="19"/>
       <c r="K4" s="166"/>
       <c r="L4" s="20"/>
@@ -29754,15 +29754,15 @@
       <c r="N4" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="P4" s="496"/>
+      <c r="P4" s="485"/>
       <c r="Q4" s="323" t="s">
         <v>217</v>
       </c>
       <c r="R4" s="506"/>
-      <c r="W4" s="478" t="s">
+      <c r="W4" s="494" t="s">
         <v>124</v>
       </c>
-      <c r="X4" s="478"/>
+      <c r="X4" s="494"/>
       <c r="Y4" s="227"/>
     </row>
     <row r="5" spans="1:25" ht="18" thickBot="1" x14ac:dyDescent="0.35">
@@ -29813,8 +29813,8 @@
         <v>0</v>
       </c>
       <c r="S5" s="325"/>
-      <c r="W5" s="478"/>
-      <c r="X5" s="478"/>
+      <c r="W5" s="494"/>
+      <c r="X5" s="494"/>
       <c r="Y5" s="233"/>
     </row>
     <row r="6" spans="1:25" ht="18" thickBot="1" x14ac:dyDescent="0.35">
@@ -30573,7 +30573,7 @@
         <v>0</v>
       </c>
       <c r="S19" s="147"/>
-      <c r="W19" s="482">
+      <c r="W19" s="498">
         <f>SUM(W6:W18)</f>
         <v>0</v>
       </c>
@@ -30623,7 +30623,7 @@
         <v>0</v>
       </c>
       <c r="S20" s="147"/>
-      <c r="W20" s="483"/>
+      <c r="W20" s="499"/>
       <c r="X20" s="268"/>
       <c r="Y20" s="233"/>
     </row>
@@ -30670,8 +30670,8 @@
         <v>0</v>
       </c>
       <c r="S21" s="147"/>
-      <c r="W21" s="484"/>
-      <c r="X21" s="484"/>
+      <c r="W21" s="500"/>
+      <c r="X21" s="500"/>
       <c r="Y21" s="233"/>
       <c r="Z21" s="128"/>
     </row>
@@ -30766,8 +30766,8 @@
         <v>0</v>
       </c>
       <c r="S23" s="147"/>
-      <c r="W23" s="485"/>
-      <c r="X23" s="485"/>
+      <c r="W23" s="501"/>
+      <c r="X23" s="501"/>
       <c r="Y23" s="233"/>
       <c r="Z23" s="128"/>
     </row>
@@ -30814,8 +30814,8 @@
         <v>0</v>
       </c>
       <c r="S24" s="147"/>
-      <c r="W24" s="485"/>
-      <c r="X24" s="485"/>
+      <c r="W24" s="501"/>
+      <c r="X24" s="501"/>
       <c r="Y24" s="233"/>
       <c r="Z24" s="128"/>
     </row>
@@ -30861,8 +30861,8 @@
       <c r="R25" s="320">
         <v>0</v>
       </c>
-      <c r="W25" s="486"/>
-      <c r="X25" s="486"/>
+      <c r="W25" s="502"/>
+      <c r="X25" s="502"/>
       <c r="Y25" s="233"/>
       <c r="Z25" s="128"/>
     </row>
@@ -30908,8 +30908,8 @@
       <c r="R26" s="320">
         <v>0</v>
       </c>
-      <c r="W26" s="486"/>
-      <c r="X26" s="486"/>
+      <c r="W26" s="502"/>
+      <c r="X26" s="502"/>
       <c r="Y26" s="233"/>
       <c r="Z26" s="128"/>
     </row>
@@ -30955,9 +30955,9 @@
       <c r="R27" s="320">
         <v>0</v>
       </c>
-      <c r="W27" s="479"/>
-      <c r="X27" s="480"/>
-      <c r="Y27" s="481"/>
+      <c r="W27" s="495"/>
+      <c r="X27" s="496"/>
+      <c r="Y27" s="497"/>
       <c r="Z27" s="128"/>
     </row>
     <row r="28" spans="1:26" ht="18" thickBot="1" x14ac:dyDescent="0.35">
@@ -31002,9 +31002,9 @@
       <c r="R28" s="320">
         <v>0</v>
       </c>
-      <c r="W28" s="480"/>
-      <c r="X28" s="480"/>
-      <c r="Y28" s="481"/>
+      <c r="W28" s="496"/>
+      <c r="X28" s="496"/>
+      <c r="Y28" s="497"/>
       <c r="Z28" s="128"/>
     </row>
     <row r="29" spans="1:26" ht="18" thickBot="1" x14ac:dyDescent="0.35">
@@ -31279,11 +31279,11 @@
       <c r="J36" s="266"/>
       <c r="K36" s="250"/>
       <c r="L36" s="44"/>
-      <c r="M36" s="497">
+      <c r="M36" s="486">
         <f>SUM(M5:M35)</f>
         <v>737462.5</v>
       </c>
-      <c r="N36" s="499">
+      <c r="N36" s="488">
         <f>SUM(N5:N35)</f>
         <v>415610</v>
       </c>
@@ -31291,7 +31291,7 @@
       <c r="P36" s="277">
         <v>0</v>
       </c>
-      <c r="Q36" s="501">
+      <c r="Q36" s="490">
         <f>SUM(Q5:Q35)</f>
         <v>1416.1199999999953</v>
       </c>
@@ -31316,13 +31316,13 @@
       <c r="L37" s="61">
         <v>16518.78</v>
       </c>
-      <c r="M37" s="498"/>
-      <c r="N37" s="500"/>
+      <c r="M37" s="487"/>
+      <c r="N37" s="489"/>
       <c r="O37" s="276"/>
       <c r="P37" s="277">
         <v>0</v>
       </c>
-      <c r="Q37" s="502"/>
+      <c r="Q37" s="491"/>
       <c r="R37" s="227" t="s">
         <v>7</v>
       </c>
@@ -31603,26 +31603,26 @@
       <c r="A52" s="98"/>
       <c r="B52" s="99"/>
       <c r="C52" s="1"/>
-      <c r="H52" s="452" t="s">
+      <c r="H52" s="463" t="s">
         <v>11</v>
       </c>
-      <c r="I52" s="453"/>
+      <c r="I52" s="464"/>
       <c r="J52" s="100"/>
-      <c r="K52" s="454">
+      <c r="K52" s="465">
         <f>I50+L50</f>
         <v>84494.68</v>
       </c>
-      <c r="L52" s="487"/>
+      <c r="L52" s="492"/>
       <c r="M52" s="272"/>
       <c r="N52" s="272"/>
       <c r="P52" s="34"/>
       <c r="Q52" s="13"/>
     </row>
     <row r="53" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="D53" s="458" t="s">
+      <c r="D53" s="469" t="s">
         <v>12</v>
       </c>
-      <c r="E53" s="458"/>
+      <c r="E53" s="469"/>
       <c r="F53" s="313">
         <f>F50-K52-C50</f>
         <v>1072952.82</v>
@@ -31631,22 +31631,22 @@
       <c r="J53" s="103"/>
     </row>
     <row r="54" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="D54" s="488" t="s">
+      <c r="D54" s="493" t="s">
         <v>95</v>
       </c>
-      <c r="E54" s="488"/>
+      <c r="E54" s="493"/>
       <c r="F54" s="111">
         <v>0</v>
       </c>
-      <c r="I54" s="459" t="s">
+      <c r="I54" s="470" t="s">
         <v>13</v>
       </c>
-      <c r="J54" s="460"/>
-      <c r="K54" s="461">
+      <c r="J54" s="471"/>
+      <c r="K54" s="472">
         <f>F56+F57+F58</f>
         <v>1072952.82</v>
       </c>
-      <c r="L54" s="461"/>
+      <c r="L54" s="472"/>
       <c r="M54" s="423"/>
       <c r="N54" s="423"/>
       <c r="O54" s="423"/>
@@ -31687,11 +31687,11 @@
         <v>15</v>
       </c>
       <c r="J56" s="109"/>
-      <c r="K56" s="463">
+      <c r="K56" s="474">
         <f>-C4</f>
         <v>-1149740.4099999999</v>
       </c>
-      <c r="L56" s="464"/>
+      <c r="L56" s="475"/>
     </row>
     <row r="57" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D57" s="110" t="s">
@@ -31706,22 +31706,22 @@
     </row>
     <row r="58" spans="1:17" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C58" s="112"/>
-      <c r="D58" s="441" t="s">
+      <c r="D58" s="452" t="s">
         <v>18</v>
       </c>
-      <c r="E58" s="442"/>
+      <c r="E58" s="453"/>
       <c r="F58" s="113">
         <v>0</v>
       </c>
-      <c r="I58" s="443" t="s">
+      <c r="I58" s="454" t="s">
         <v>198</v>
       </c>
-      <c r="J58" s="444"/>
-      <c r="K58" s="445">
+      <c r="J58" s="455"/>
+      <c r="K58" s="456">
         <f>K54+K56</f>
         <v>-76787.589999999851</v>
       </c>
-      <c r="L58" s="445"/>
+      <c r="L58" s="456"/>
     </row>
     <row r="59" spans="1:17" ht="17.25" x14ac:dyDescent="0.3">
       <c r="C59" s="114"/>
@@ -31865,20 +31865,6 @@
     </row>
   </sheetData>
   <mergeCells count="29">
-    <mergeCell ref="W26:X26"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:M1"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="H3:I3"/>
-    <mergeCell ref="P3:P4"/>
-    <mergeCell ref="R3:R4"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="H4:I4"/>
-    <mergeCell ref="W4:X5"/>
-    <mergeCell ref="W19:W20"/>
-    <mergeCell ref="W21:X21"/>
-    <mergeCell ref="W23:X24"/>
-    <mergeCell ref="W25:X25"/>
     <mergeCell ref="D58:E58"/>
     <mergeCell ref="I58:J58"/>
     <mergeCell ref="K58:L58"/>
@@ -31894,6 +31880,20 @@
     <mergeCell ref="I54:J54"/>
     <mergeCell ref="K54:L54"/>
     <mergeCell ref="K56:L56"/>
+    <mergeCell ref="W26:X26"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:M1"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="P3:P4"/>
+    <mergeCell ref="R3:R4"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="H4:I4"/>
+    <mergeCell ref="W4:X5"/>
+    <mergeCell ref="W19:W20"/>
+    <mergeCell ref="W21:X21"/>
+    <mergeCell ref="W23:X24"/>
+    <mergeCell ref="W25:X25"/>
   </mergeCells>
   <pageMargins left="0.23" right="0.23" top="0.4" bottom="0.28000000000000003" header="0.3" footer="0.3"/>
   <pageSetup orientation="landscape" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
CIERRE  3 MAR 22
</commit_message>
<xml_diff>
--- a/01 DOCUEMENTOS/CENTRAL  ARCHIVO   2 0 2 2/CENTRAL #02  FEBRERO 2022/BALANCE    ZAVALETA   FEBRERO     2022 VALIDA.xlsx
+++ b/01 DOCUEMENTOS/CENTRAL  ARCHIVO   2 0 2 2/CENTRAL #02  FEBRERO 2022/BALANCE    ZAVALETA   FEBRERO     2022 VALIDA.xlsx
@@ -373,7 +373,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="925" uniqueCount="452">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="935" uniqueCount="460">
   <si>
     <t>COMPRAS</t>
   </si>
@@ -1729,6 +1729,30 @@
   </si>
   <si>
     <t>LONGANIZA-JAMON-´POLLO-</t>
+  </si>
+  <si>
+    <t>LONGANIZA-QUESOS-SALCHICHONERIA</t>
+  </si>
+  <si>
+    <t>Odelpa</t>
+  </si>
+  <si>
+    <t>CHORIZO-QUESOS-POLLO</t>
+  </si>
+  <si>
+    <t>Odelpa Y zav</t>
+  </si>
+  <si>
+    <t>POLLO-CHISTORRA-QUESOS</t>
+  </si>
+  <si>
+    <t>NOMINA #9</t>
+  </si>
+  <si>
+    <t>SEMANA # 9</t>
+  </si>
+  <si>
+    <t>ENCHILADA</t>
   </si>
 </sst>
 </file>
@@ -1744,7 +1768,7 @@
     <numFmt numFmtId="167" formatCode="[$$-80A]#,##0.00;\-[$$-80A]#,##0.00"/>
     <numFmt numFmtId="168" formatCode="[$-C0A]d\-mmm\-yyyy;@"/>
   </numFmts>
-  <fonts count="54" x14ac:knownFonts="1">
+  <fonts count="56" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2167,6 +2191,22 @@
       <u/>
       <sz val="18"/>
       <color rgb="FFC00000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="8"/>
+      <color rgb="FF800000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF800000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -3586,7 +3626,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="548">
+  <cellXfs count="559">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="44" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
@@ -4480,6 +4520,39 @@
     </xf>
     <xf numFmtId="44" fontId="47" fillId="3" borderId="26" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="44" fontId="3" fillId="3" borderId="26" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="40" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="40" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="4" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="27" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -4552,45 +4625,60 @@
     <xf numFmtId="44" fontId="12" fillId="0" borderId="49" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="4" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="1" fontId="43" fillId="6" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="1" fontId="43" fillId="6" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="44" fontId="13" fillId="0" borderId="57" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="13" fillId="0" borderId="77" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="13" fillId="0" borderId="58" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="13" fillId="0" borderId="33" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="13" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="13" fillId="0" borderId="59" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="16" fillId="3" borderId="69" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="16" fillId="3" borderId="71" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="2" fillId="3" borderId="70" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="2" fillId="3" borderId="72" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="41" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="41" fillId="3" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="10" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="44" fontId="13" fillId="9" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -4618,54 +4706,6 @@
     <xf numFmtId="7" fontId="11" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="10" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="44" fontId="13" fillId="0" borderId="57" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="13" fillId="0" borderId="77" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="13" fillId="0" borderId="58" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="13" fillId="0" borderId="33" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="13" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="13" fillId="0" borderId="59" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="44" fontId="16" fillId="3" borderId="69" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="16" fillId="3" borderId="71" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="2" fillId="3" borderId="70" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="2" fillId="3" borderId="72" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="41" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="41" fillId="3" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="44" fontId="3" fillId="3" borderId="74" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -4793,6 +4833,27 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="11" fillId="14" borderId="99" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="2" fillId="9" borderId="24" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="3" fillId="0" borderId="73" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="2" fillId="17" borderId="85" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="54" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="44" fontId="2" fillId="9" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="44" fontId="55" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="11" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="11" fillId="3" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="7" fontId="13" fillId="6" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="7" fontId="13" fillId="6" borderId="16" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -4804,11 +4865,11 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FF800000"/>
+      <color rgb="FF99CCFF"/>
       <color rgb="FF0000FF"/>
       <color rgb="FFCCFF66"/>
-      <color rgb="FF99CCFF"/>
       <color rgb="FF66FFFF"/>
-      <color rgb="FF800000"/>
       <color rgb="FF6600FF"/>
       <color rgb="FF00FF00"/>
       <color rgb="FF00FF99"/>
@@ -7364,23 +7425,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B1" s="467"/>
-      <c r="C1" s="469" t="s">
+      <c r="B1" s="443"/>
+      <c r="C1" s="445" t="s">
         <v>25</v>
       </c>
-      <c r="D1" s="470"/>
-      <c r="E1" s="470"/>
-      <c r="F1" s="470"/>
-      <c r="G1" s="470"/>
-      <c r="H1" s="470"/>
-      <c r="I1" s="470"/>
-      <c r="J1" s="470"/>
-      <c r="K1" s="470"/>
-      <c r="L1" s="470"/>
-      <c r="M1" s="470"/>
+      <c r="D1" s="446"/>
+      <c r="E1" s="446"/>
+      <c r="F1" s="446"/>
+      <c r="G1" s="446"/>
+      <c r="H1" s="446"/>
+      <c r="I1" s="446"/>
+      <c r="J1" s="446"/>
+      <c r="K1" s="446"/>
+      <c r="L1" s="446"/>
+      <c r="M1" s="446"/>
     </row>
     <row r="2" spans="1:19" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="468"/>
+      <c r="B2" s="444"/>
       <c r="C2" s="3"/>
       <c r="H2" s="5"/>
       <c r="I2" s="6"/>
@@ -7390,17 +7451,17 @@
       <c r="N2" s="9"/>
     </row>
     <row r="3" spans="1:19" ht="21.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="471" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="472"/>
+      <c r="B3" s="447" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="448"/>
       <c r="D3" s="10"/>
       <c r="E3" s="11"/>
       <c r="F3" s="11"/>
-      <c r="H3" s="473" t="s">
+      <c r="H3" s="449" t="s">
         <v>26</v>
       </c>
-      <c r="I3" s="473"/>
+      <c r="I3" s="449"/>
       <c r="K3" s="165"/>
       <c r="L3" s="13"/>
       <c r="M3" s="14"/>
@@ -7414,14 +7475,14 @@
         <v>0</v>
       </c>
       <c r="D4" s="18"/>
-      <c r="E4" s="474" t="s">
+      <c r="E4" s="450" t="s">
         <v>2</v>
       </c>
-      <c r="F4" s="475"/>
-      <c r="H4" s="476" t="s">
+      <c r="F4" s="451"/>
+      <c r="H4" s="452" t="s">
         <v>3</v>
       </c>
-      <c r="I4" s="477"/>
+      <c r="I4" s="453"/>
       <c r="J4" s="19"/>
       <c r="K4" s="166"/>
       <c r="L4" s="20"/>
@@ -7431,10 +7492,10 @@
       <c r="N4" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="P4" s="448" t="s">
+      <c r="P4" s="459" t="s">
         <v>6</v>
       </c>
-      <c r="Q4" s="449"/>
+      <c r="Q4" s="460"/>
     </row>
     <row r="5" spans="1:19" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="23" t="s">
@@ -8875,11 +8936,11 @@
       <c r="J39" s="60"/>
       <c r="K39" s="177"/>
       <c r="L39" s="61"/>
-      <c r="M39" s="450">
+      <c r="M39" s="461">
         <f>SUM(M5:M38)</f>
         <v>247061</v>
       </c>
-      <c r="N39" s="452">
+      <c r="N39" s="463">
         <f>SUM(N5:N38)</f>
         <v>172863</v>
       </c>
@@ -8905,8 +8966,8 @@
       <c r="J40" s="60"/>
       <c r="K40" s="41"/>
       <c r="L40" s="61"/>
-      <c r="M40" s="451"/>
-      <c r="N40" s="453"/>
+      <c r="M40" s="462"/>
+      <c r="N40" s="464"/>
       <c r="P40" s="34"/>
       <c r="Q40" s="9"/>
     </row>
@@ -9121,29 +9182,29 @@
       <c r="A52" s="98"/>
       <c r="B52" s="99"/>
       <c r="C52" s="1"/>
-      <c r="H52" s="454" t="s">
+      <c r="H52" s="465" t="s">
         <v>11</v>
       </c>
-      <c r="I52" s="455"/>
+      <c r="I52" s="466"/>
       <c r="J52" s="100"/>
-      <c r="K52" s="456">
+      <c r="K52" s="467">
         <f>I50+L50</f>
         <v>53873.49</v>
       </c>
-      <c r="L52" s="457"/>
-      <c r="M52" s="458">
+      <c r="L52" s="468"/>
+      <c r="M52" s="469">
         <f>N39+M39</f>
         <v>419924</v>
       </c>
-      <c r="N52" s="459"/>
+      <c r="N52" s="470"/>
       <c r="P52" s="34"/>
       <c r="Q52" s="9"/>
     </row>
     <row r="53" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="D53" s="460" t="s">
+      <c r="D53" s="471" t="s">
         <v>12</v>
       </c>
-      <c r="E53" s="460"/>
+      <c r="E53" s="471"/>
       <c r="F53" s="101">
         <f>F50-K52-C50</f>
         <v>471038.61</v>
@@ -9154,22 +9215,22 @@
       <c r="Q53" s="9"/>
     </row>
     <row r="54" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="D54" s="460" t="s">
+      <c r="D54" s="471" t="s">
         <v>95</v>
       </c>
-      <c r="E54" s="460"/>
+      <c r="E54" s="471"/>
       <c r="F54" s="96">
         <v>-549976.4</v>
       </c>
-      <c r="I54" s="461" t="s">
+      <c r="I54" s="472" t="s">
         <v>13</v>
       </c>
-      <c r="J54" s="462"/>
-      <c r="K54" s="463">
+      <c r="J54" s="473"/>
+      <c r="K54" s="474">
         <f>F56+F57+F58</f>
         <v>-24577.400000000023</v>
       </c>
-      <c r="L54" s="464"/>
+      <c r="L54" s="475"/>
       <c r="P54" s="34"/>
       <c r="Q54" s="9"/>
     </row>
@@ -9202,11 +9263,11 @@
         <v>15</v>
       </c>
       <c r="J56" s="109"/>
-      <c r="K56" s="465">
+      <c r="K56" s="476">
         <f>-C4</f>
         <v>0</v>
       </c>
-      <c r="L56" s="466"/>
+      <c r="L56" s="477"/>
     </row>
     <row r="57" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D57" s="110" t="s">
@@ -9223,22 +9284,22 @@
       <c r="C58" s="112">
         <v>44507</v>
       </c>
-      <c r="D58" s="443" t="s">
+      <c r="D58" s="454" t="s">
         <v>18</v>
       </c>
-      <c r="E58" s="444"/>
+      <c r="E58" s="455"/>
       <c r="F58" s="113">
         <v>567389.35</v>
       </c>
-      <c r="I58" s="445" t="s">
+      <c r="I58" s="456" t="s">
         <v>97</v>
       </c>
-      <c r="J58" s="446"/>
-      <c r="K58" s="447">
+      <c r="J58" s="457"/>
+      <c r="K58" s="458">
         <f>K54+K56</f>
         <v>-24577.400000000023</v>
       </c>
-      <c r="L58" s="447"/>
+      <c r="L58" s="458"/>
     </row>
     <row r="59" spans="1:17" ht="17.25" x14ac:dyDescent="0.3">
       <c r="C59" s="114"/>
@@ -9382,12 +9443,6 @@
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:M1"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="H3:I3"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="H4:I4"/>
     <mergeCell ref="D58:E58"/>
     <mergeCell ref="I58:J58"/>
     <mergeCell ref="K58:L58"/>
@@ -9402,6 +9457,12 @@
     <mergeCell ref="I54:J54"/>
     <mergeCell ref="K54:L54"/>
     <mergeCell ref="K56:L56"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:M1"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="H4:I4"/>
   </mergeCells>
   <pageMargins left="0.39370078740157483" right="0.15748031496062992" top="0.35433070866141736" bottom="0.31496062992125984" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup scale="75" orientation="landscape" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -14570,23 +14631,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:25" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B1" s="467"/>
-      <c r="C1" s="469" t="s">
+      <c r="B1" s="443"/>
+      <c r="C1" s="445" t="s">
         <v>208</v>
       </c>
-      <c r="D1" s="470"/>
-      <c r="E1" s="470"/>
-      <c r="F1" s="470"/>
-      <c r="G1" s="470"/>
-      <c r="H1" s="470"/>
-      <c r="I1" s="470"/>
-      <c r="J1" s="470"/>
-      <c r="K1" s="470"/>
-      <c r="L1" s="470"/>
-      <c r="M1" s="470"/>
+      <c r="D1" s="446"/>
+      <c r="E1" s="446"/>
+      <c r="F1" s="446"/>
+      <c r="G1" s="446"/>
+      <c r="H1" s="446"/>
+      <c r="I1" s="446"/>
+      <c r="J1" s="446"/>
+      <c r="K1" s="446"/>
+      <c r="L1" s="446"/>
+      <c r="M1" s="446"/>
     </row>
     <row r="2" spans="1:25" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="468"/>
+      <c r="B2" s="444"/>
       <c r="C2" s="3"/>
       <c r="H2" s="5"/>
       <c r="I2" s="6"/>
@@ -14596,21 +14657,21 @@
       <c r="N2" s="9"/>
     </row>
     <row r="3" spans="1:25" ht="21.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="471" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="472"/>
+      <c r="B3" s="447" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="448"/>
       <c r="D3" s="10"/>
       <c r="E3" s="11"/>
       <c r="F3" s="11"/>
-      <c r="H3" s="473" t="s">
+      <c r="H3" s="449" t="s">
         <v>26</v>
       </c>
-      <c r="I3" s="473"/>
+      <c r="I3" s="449"/>
       <c r="K3" s="165"/>
       <c r="L3" s="13"/>
       <c r="M3" s="14"/>
-      <c r="P3" s="497" t="s">
+      <c r="P3" s="486" t="s">
         <v>6</v>
       </c>
     </row>
@@ -14625,14 +14686,14 @@
       <c r="D4" s="18">
         <v>44507</v>
       </c>
-      <c r="E4" s="474" t="s">
+      <c r="E4" s="450" t="s">
         <v>2</v>
       </c>
-      <c r="F4" s="475"/>
-      <c r="H4" s="476" t="s">
+      <c r="F4" s="451"/>
+      <c r="H4" s="452" t="s">
         <v>3</v>
       </c>
-      <c r="I4" s="477"/>
+      <c r="I4" s="453"/>
       <c r="J4" s="19"/>
       <c r="K4" s="166"/>
       <c r="L4" s="20"/>
@@ -14642,14 +14703,14 @@
       <c r="N4" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="P4" s="498"/>
+      <c r="P4" s="487"/>
       <c r="Q4" s="286" t="s">
         <v>209</v>
       </c>
-      <c r="W4" s="480" t="s">
+      <c r="W4" s="496" t="s">
         <v>124</v>
       </c>
-      <c r="X4" s="480"/>
+      <c r="X4" s="496"/>
       <c r="Y4" s="227"/>
     </row>
     <row r="5" spans="1:25" ht="18" thickBot="1" x14ac:dyDescent="0.35">
@@ -14700,8 +14761,8 @@
         <f>20000+7936</f>
         <v>27936</v>
       </c>
-      <c r="W5" s="480"/>
-      <c r="X5" s="480"/>
+      <c r="W5" s="496"/>
+      <c r="X5" s="496"/>
       <c r="Y5" s="233"/>
     </row>
     <row r="6" spans="1:25" ht="18" thickBot="1" x14ac:dyDescent="0.35">
@@ -15472,7 +15533,7 @@
         <v>26370</v>
       </c>
       <c r="S19" s="147"/>
-      <c r="W19" s="484">
+      <c r="W19" s="500">
         <f>SUM(W6:W18)</f>
         <v>935136</v>
       </c>
@@ -15524,7 +15585,7 @@
         <v>16395.830000000002</v>
       </c>
       <c r="S20" s="147"/>
-      <c r="W20" s="485"/>
+      <c r="W20" s="501"/>
       <c r="X20" s="268"/>
       <c r="Y20" s="233"/>
     </row>
@@ -15573,8 +15634,8 @@
         <v>19188.82</v>
       </c>
       <c r="S21" s="147"/>
-      <c r="W21" s="486"/>
-      <c r="X21" s="486"/>
+      <c r="W21" s="502"/>
+      <c r="X21" s="502"/>
       <c r="Y21" s="233"/>
       <c r="Z21" s="128"/>
     </row>
@@ -15675,8 +15736,8 @@
         <v>45217.29</v>
       </c>
       <c r="S23" s="147"/>
-      <c r="W23" s="487"/>
-      <c r="X23" s="487"/>
+      <c r="W23" s="503"/>
+      <c r="X23" s="503"/>
       <c r="Y23" s="233"/>
       <c r="Z23" s="128"/>
     </row>
@@ -15730,8 +15791,8 @@
         <v>23159.17</v>
       </c>
       <c r="S24" s="147"/>
-      <c r="W24" s="487"/>
-      <c r="X24" s="487"/>
+      <c r="W24" s="503"/>
+      <c r="X24" s="503"/>
       <c r="Y24" s="233"/>
       <c r="Z24" s="128"/>
     </row>
@@ -15777,8 +15838,8 @@
       <c r="R25" s="285">
         <v>28952</v>
       </c>
-      <c r="W25" s="488"/>
-      <c r="X25" s="488"/>
+      <c r="W25" s="504"/>
+      <c r="X25" s="504"/>
       <c r="Y25" s="233"/>
       <c r="Z25" s="128"/>
     </row>
@@ -15829,8 +15890,8 @@
       <c r="R26" s="285">
         <v>21771.5</v>
       </c>
-      <c r="W26" s="488"/>
-      <c r="X26" s="488"/>
+      <c r="W26" s="504"/>
+      <c r="X26" s="504"/>
       <c r="Y26" s="233"/>
       <c r="Z26" s="128"/>
     </row>
@@ -15878,9 +15939,9 @@
       <c r="R27" s="285">
         <v>14637</v>
       </c>
-      <c r="W27" s="481"/>
-      <c r="X27" s="482"/>
-      <c r="Y27" s="483"/>
+      <c r="W27" s="497"/>
+      <c r="X27" s="498"/>
+      <c r="Y27" s="499"/>
       <c r="Z27" s="128"/>
     </row>
     <row r="28" spans="1:26" ht="18" thickBot="1" x14ac:dyDescent="0.35">
@@ -15930,9 +15991,9 @@
       <c r="R28" s="285">
         <v>0</v>
       </c>
-      <c r="W28" s="482"/>
-      <c r="X28" s="482"/>
-      <c r="Y28" s="483"/>
+      <c r="W28" s="498"/>
+      <c r="X28" s="498"/>
+      <c r="Y28" s="499"/>
       <c r="Z28" s="128"/>
     </row>
     <row r="29" spans="1:26" ht="18" thickBot="1" x14ac:dyDescent="0.35">
@@ -16267,11 +16328,11 @@
       <c r="L36" s="44">
         <v>5940</v>
       </c>
-      <c r="M36" s="499">
+      <c r="M36" s="488">
         <f>SUM(M5:M35)</f>
         <v>321168.83</v>
       </c>
-      <c r="N36" s="501">
+      <c r="N36" s="490">
         <f>SUM(N5:N35)</f>
         <v>467016</v>
       </c>
@@ -16279,7 +16340,7 @@
       <c r="P36" s="277">
         <v>0</v>
       </c>
-      <c r="Q36" s="503">
+      <c r="Q36" s="492">
         <f>SUM(Q5:Q35)</f>
         <v>-637069.14000000013</v>
       </c>
@@ -16314,13 +16375,13 @@
       <c r="L37" s="61">
         <v>7929.62</v>
       </c>
-      <c r="M37" s="500"/>
-      <c r="N37" s="502"/>
+      <c r="M37" s="489"/>
+      <c r="N37" s="491"/>
       <c r="O37" s="276"/>
       <c r="P37" s="277">
         <v>0</v>
       </c>
-      <c r="Q37" s="504"/>
+      <c r="Q37" s="493"/>
     </row>
     <row r="38" spans="1:18" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A38" s="23"/>
@@ -16610,26 +16671,26 @@
       <c r="A52" s="98"/>
       <c r="B52" s="99"/>
       <c r="C52" s="1"/>
-      <c r="H52" s="454" t="s">
+      <c r="H52" s="465" t="s">
         <v>11</v>
       </c>
-      <c r="I52" s="455"/>
+      <c r="I52" s="466"/>
       <c r="J52" s="100"/>
-      <c r="K52" s="456">
+      <c r="K52" s="467">
         <f>I50+L50</f>
         <v>71911.59</v>
       </c>
-      <c r="L52" s="489"/>
+      <c r="L52" s="494"/>
       <c r="M52" s="272"/>
       <c r="N52" s="272"/>
       <c r="P52" s="34"/>
       <c r="Q52" s="13"/>
     </row>
     <row r="53" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D53" s="460" t="s">
+      <c r="D53" s="471" t="s">
         <v>12</v>
       </c>
-      <c r="E53" s="460"/>
+      <c r="E53" s="471"/>
       <c r="F53" s="313">
         <f>F50-K52-C50</f>
         <v>-25952.549999999814</v>
@@ -16638,29 +16699,29 @@
       <c r="J53" s="103"/>
     </row>
     <row r="54" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="D54" s="490" t="s">
+      <c r="D54" s="495" t="s">
         <v>95</v>
       </c>
-      <c r="E54" s="490"/>
+      <c r="E54" s="495"/>
       <c r="F54" s="111">
         <v>-706888.38</v>
       </c>
-      <c r="I54" s="461" t="s">
+      <c r="I54" s="472" t="s">
         <v>13</v>
       </c>
-      <c r="J54" s="462"/>
-      <c r="K54" s="463">
+      <c r="J54" s="473"/>
+      <c r="K54" s="474">
         <f>F56+F57+F58</f>
         <v>1308778.3500000003</v>
       </c>
-      <c r="L54" s="463"/>
-      <c r="M54" s="491" t="s">
+      <c r="L54" s="474"/>
+      <c r="M54" s="480" t="s">
         <v>211</v>
       </c>
-      <c r="N54" s="492"/>
-      <c r="O54" s="492"/>
-      <c r="P54" s="492"/>
-      <c r="Q54" s="493"/>
+      <c r="N54" s="481"/>
+      <c r="O54" s="481"/>
+      <c r="P54" s="481"/>
+      <c r="Q54" s="482"/>
     </row>
     <row r="55" spans="1:17" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D55" s="314" t="s">
@@ -16674,11 +16735,11 @@
       <c r="J55" s="106"/>
       <c r="K55" s="178"/>
       <c r="L55" s="107"/>
-      <c r="M55" s="494"/>
-      <c r="N55" s="495"/>
-      <c r="O55" s="495"/>
-      <c r="P55" s="495"/>
-      <c r="Q55" s="496"/>
+      <c r="M55" s="483"/>
+      <c r="N55" s="484"/>
+      <c r="O55" s="484"/>
+      <c r="P55" s="484"/>
+      <c r="Q55" s="485"/>
     </row>
     <row r="56" spans="1:17" ht="19.5" thickTop="1" x14ac:dyDescent="0.3">
       <c r="C56" s="4" t="s">
@@ -16696,11 +16757,11 @@
         <v>15</v>
       </c>
       <c r="J56" s="109"/>
-      <c r="K56" s="465">
+      <c r="K56" s="476">
         <f>-C4</f>
         <v>-567389.35</v>
       </c>
-      <c r="L56" s="466"/>
+      <c r="L56" s="477"/>
     </row>
     <row r="57" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D57" s="110" t="s">
@@ -16717,22 +16778,22 @@
       <c r="C58" s="112">
         <v>44535</v>
       </c>
-      <c r="D58" s="443" t="s">
+      <c r="D58" s="454" t="s">
         <v>18</v>
       </c>
-      <c r="E58" s="444"/>
+      <c r="E58" s="455"/>
       <c r="F58" s="113">
         <v>2142307.62</v>
       </c>
-      <c r="I58" s="445" t="s">
+      <c r="I58" s="456" t="s">
         <v>198</v>
       </c>
-      <c r="J58" s="446"/>
-      <c r="K58" s="447">
+      <c r="J58" s="457"/>
+      <c r="K58" s="458">
         <f>K54+K56</f>
         <v>741389.00000000035</v>
       </c>
-      <c r="L58" s="447"/>
+      <c r="L58" s="458"/>
     </row>
     <row r="59" spans="1:17" ht="17.25" x14ac:dyDescent="0.3">
       <c r="C59" s="114"/>
@@ -16876,17 +16937,14 @@
     </row>
   </sheetData>
   <mergeCells count="29">
-    <mergeCell ref="M54:Q55"/>
-    <mergeCell ref="P3:P4"/>
-    <mergeCell ref="M36:M37"/>
-    <mergeCell ref="N36:N37"/>
-    <mergeCell ref="Q36:Q37"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:M1"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="H3:I3"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="H4:I4"/>
+    <mergeCell ref="W4:X5"/>
+    <mergeCell ref="W27:X28"/>
+    <mergeCell ref="Y27:Y28"/>
+    <mergeCell ref="W19:W20"/>
+    <mergeCell ref="W21:X21"/>
+    <mergeCell ref="W23:X24"/>
+    <mergeCell ref="W25:X25"/>
+    <mergeCell ref="W26:X26"/>
     <mergeCell ref="D58:E58"/>
     <mergeCell ref="I58:J58"/>
     <mergeCell ref="K58:L58"/>
@@ -16897,14 +16955,17 @@
     <mergeCell ref="I54:J54"/>
     <mergeCell ref="K54:L54"/>
     <mergeCell ref="K56:L56"/>
-    <mergeCell ref="W4:X5"/>
-    <mergeCell ref="W27:X28"/>
-    <mergeCell ref="Y27:Y28"/>
-    <mergeCell ref="W19:W20"/>
-    <mergeCell ref="W21:X21"/>
-    <mergeCell ref="W23:X24"/>
-    <mergeCell ref="W25:X25"/>
-    <mergeCell ref="W26:X26"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:M1"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="H4:I4"/>
+    <mergeCell ref="M54:Q55"/>
+    <mergeCell ref="P3:P4"/>
+    <mergeCell ref="M36:M37"/>
+    <mergeCell ref="N36:N37"/>
+    <mergeCell ref="Q36:Q37"/>
   </mergeCells>
   <pageMargins left="0.15748031496062992" right="0.15748031496062992" top="0.27559055118110237" bottom="0.27559055118110237" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup scale="68" orientation="landscape" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -19647,23 +19708,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:25" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B1" s="467"/>
-      <c r="C1" s="469" t="s">
+      <c r="B1" s="443"/>
+      <c r="C1" s="445" t="s">
         <v>208</v>
       </c>
-      <c r="D1" s="470"/>
-      <c r="E1" s="470"/>
-      <c r="F1" s="470"/>
-      <c r="G1" s="470"/>
-      <c r="H1" s="470"/>
-      <c r="I1" s="470"/>
-      <c r="J1" s="470"/>
-      <c r="K1" s="470"/>
-      <c r="L1" s="470"/>
-      <c r="M1" s="470"/>
+      <c r="D1" s="446"/>
+      <c r="E1" s="446"/>
+      <c r="F1" s="446"/>
+      <c r="G1" s="446"/>
+      <c r="H1" s="446"/>
+      <c r="I1" s="446"/>
+      <c r="J1" s="446"/>
+      <c r="K1" s="446"/>
+      <c r="L1" s="446"/>
+      <c r="M1" s="446"/>
     </row>
     <row r="2" spans="1:25" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="468"/>
+      <c r="B2" s="444"/>
       <c r="C2" s="3"/>
       <c r="H2" s="5"/>
       <c r="I2" s="6"/>
@@ -19673,21 +19734,21 @@
       <c r="N2" s="9"/>
     </row>
     <row r="3" spans="1:25" ht="21.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="471" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="472"/>
+      <c r="B3" s="447" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="448"/>
       <c r="D3" s="10"/>
       <c r="E3" s="11"/>
       <c r="F3" s="11"/>
-      <c r="H3" s="473" t="s">
+      <c r="H3" s="449" t="s">
         <v>26</v>
       </c>
-      <c r="I3" s="473"/>
+      <c r="I3" s="449"/>
       <c r="K3" s="165"/>
       <c r="L3" s="13"/>
       <c r="M3" s="14"/>
-      <c r="P3" s="497" t="s">
+      <c r="P3" s="486" t="s">
         <v>6</v>
       </c>
       <c r="R3" s="507" t="s">
@@ -19705,14 +19766,14 @@
       <c r="D4" s="18">
         <v>44507</v>
       </c>
-      <c r="E4" s="474" t="s">
+      <c r="E4" s="450" t="s">
         <v>2</v>
       </c>
-      <c r="F4" s="475"/>
-      <c r="H4" s="476" t="s">
+      <c r="F4" s="451"/>
+      <c r="H4" s="452" t="s">
         <v>3</v>
       </c>
-      <c r="I4" s="477"/>
+      <c r="I4" s="453"/>
       <c r="J4" s="19"/>
       <c r="K4" s="166"/>
       <c r="L4" s="20"/>
@@ -19722,15 +19783,15 @@
       <c r="N4" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="P4" s="498"/>
+      <c r="P4" s="487"/>
       <c r="Q4" s="323" t="s">
         <v>217</v>
       </c>
       <c r="R4" s="508"/>
-      <c r="W4" s="480" t="s">
+      <c r="W4" s="496" t="s">
         <v>124</v>
       </c>
-      <c r="X4" s="480"/>
+      <c r="X4" s="496"/>
       <c r="Y4" s="227"/>
     </row>
     <row r="5" spans="1:25" ht="18" thickBot="1" x14ac:dyDescent="0.35">
@@ -19791,8 +19852,8 @@
       <c r="S5" s="325" t="s">
         <v>213</v>
       </c>
-      <c r="W5" s="480"/>
-      <c r="X5" s="480"/>
+      <c r="W5" s="496"/>
+      <c r="X5" s="496"/>
       <c r="Y5" s="233"/>
     </row>
     <row r="6" spans="1:25" ht="18" thickBot="1" x14ac:dyDescent="0.35">
@@ -20549,7 +20610,7 @@
         <v>0</v>
       </c>
       <c r="S19" s="147"/>
-      <c r="W19" s="484">
+      <c r="W19" s="500">
         <f>SUM(W6:W18)</f>
         <v>0</v>
       </c>
@@ -20601,7 +20662,7 @@
         <v>0</v>
       </c>
       <c r="S20" s="147"/>
-      <c r="W20" s="485"/>
+      <c r="W20" s="501"/>
       <c r="X20" s="268"/>
       <c r="Y20" s="233"/>
     </row>
@@ -20650,8 +20711,8 @@
         <v>0</v>
       </c>
       <c r="S21" s="147"/>
-      <c r="W21" s="486"/>
-      <c r="X21" s="486"/>
+      <c r="W21" s="502"/>
+      <c r="X21" s="502"/>
       <c r="Y21" s="233"/>
       <c r="Z21" s="128"/>
     </row>
@@ -20752,8 +20813,8 @@
         <v>0</v>
       </c>
       <c r="S23" s="147"/>
-      <c r="W23" s="487"/>
-      <c r="X23" s="487"/>
+      <c r="W23" s="503"/>
+      <c r="X23" s="503"/>
       <c r="Y23" s="233"/>
       <c r="Z23" s="128"/>
     </row>
@@ -20804,8 +20865,8 @@
         <v>0</v>
       </c>
       <c r="S24" s="147"/>
-      <c r="W24" s="487"/>
-      <c r="X24" s="487"/>
+      <c r="W24" s="503"/>
+      <c r="X24" s="503"/>
       <c r="Y24" s="233"/>
       <c r="Z24" s="128"/>
     </row>
@@ -20851,8 +20912,8 @@
       <c r="R25" s="320">
         <v>0</v>
       </c>
-      <c r="W25" s="488"/>
-      <c r="X25" s="488"/>
+      <c r="W25" s="504"/>
+      <c r="X25" s="504"/>
       <c r="Y25" s="233"/>
       <c r="Z25" s="128"/>
     </row>
@@ -20900,8 +20961,8 @@
       <c r="R26" s="320">
         <v>0</v>
       </c>
-      <c r="W26" s="488"/>
-      <c r="X26" s="488"/>
+      <c r="W26" s="504"/>
+      <c r="X26" s="504"/>
       <c r="Y26" s="233"/>
       <c r="Z26" s="128"/>
     </row>
@@ -20961,9 +21022,9 @@
       <c r="V27" t="s">
         <v>240</v>
       </c>
-      <c r="W27" s="481"/>
-      <c r="X27" s="482"/>
-      <c r="Y27" s="483"/>
+      <c r="W27" s="497"/>
+      <c r="X27" s="498"/>
+      <c r="Y27" s="499"/>
       <c r="Z27" s="128"/>
     </row>
     <row r="28" spans="1:26" ht="18" thickBot="1" x14ac:dyDescent="0.35">
@@ -21017,9 +21078,9 @@
       <c r="V28" t="s">
         <v>240</v>
       </c>
-      <c r="W28" s="482"/>
-      <c r="X28" s="482"/>
-      <c r="Y28" s="483"/>
+      <c r="W28" s="498"/>
+      <c r="X28" s="498"/>
+      <c r="Y28" s="499"/>
       <c r="Z28" s="128"/>
     </row>
     <row r="29" spans="1:26" ht="18" thickBot="1" x14ac:dyDescent="0.35">
@@ -21335,11 +21396,11 @@
       <c r="J36" s="266"/>
       <c r="K36" s="250"/>
       <c r="L36" s="44"/>
-      <c r="M36" s="499">
+      <c r="M36" s="488">
         <f>SUM(M5:M35)</f>
         <v>1077791.3</v>
       </c>
-      <c r="N36" s="501">
+      <c r="N36" s="490">
         <f>SUM(N5:N35)</f>
         <v>936398</v>
       </c>
@@ -21347,7 +21408,7 @@
       <c r="P36" s="277">
         <v>0</v>
       </c>
-      <c r="Q36" s="503">
+      <c r="Q36" s="492">
         <f>SUM(Q5:Q35)</f>
         <v>-14262.940000000002</v>
       </c>
@@ -21366,13 +21427,13 @@
       <c r="J37" s="60"/>
       <c r="K37" s="41"/>
       <c r="L37" s="61"/>
-      <c r="M37" s="500"/>
-      <c r="N37" s="502"/>
+      <c r="M37" s="489"/>
+      <c r="N37" s="491"/>
       <c r="O37" s="276"/>
       <c r="P37" s="277">
         <v>0</v>
       </c>
-      <c r="Q37" s="504"/>
+      <c r="Q37" s="493"/>
     </row>
     <row r="38" spans="1:18" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A38" s="23"/>
@@ -21646,26 +21707,26 @@
       <c r="A52" s="98"/>
       <c r="B52" s="99"/>
       <c r="C52" s="1"/>
-      <c r="H52" s="454" t="s">
+      <c r="H52" s="465" t="s">
         <v>11</v>
       </c>
-      <c r="I52" s="455"/>
+      <c r="I52" s="466"/>
       <c r="J52" s="100"/>
-      <c r="K52" s="456">
+      <c r="K52" s="467">
         <f>I50+L50</f>
         <v>90750.75</v>
       </c>
-      <c r="L52" s="489"/>
+      <c r="L52" s="494"/>
       <c r="M52" s="272"/>
       <c r="N52" s="272"/>
       <c r="P52" s="34"/>
       <c r="Q52" s="13"/>
     </row>
     <row r="53" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D53" s="460" t="s">
+      <c r="D53" s="471" t="s">
         <v>12</v>
       </c>
-      <c r="E53" s="460"/>
+      <c r="E53" s="471"/>
       <c r="F53" s="313">
         <f>F50-K52-C50</f>
         <v>1739855.03</v>
@@ -21674,29 +21735,29 @@
       <c r="J53" s="103"/>
     </row>
     <row r="54" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="D54" s="490" t="s">
+      <c r="D54" s="495" t="s">
         <v>95</v>
       </c>
-      <c r="E54" s="490"/>
+      <c r="E54" s="495"/>
       <c r="F54" s="111">
         <v>-1567070.66</v>
       </c>
-      <c r="I54" s="461" t="s">
+      <c r="I54" s="472" t="s">
         <v>13</v>
       </c>
-      <c r="J54" s="462"/>
-      <c r="K54" s="463">
+      <c r="J54" s="473"/>
+      <c r="K54" s="474">
         <f>F56+F57+F58</f>
         <v>703192.8600000001</v>
       </c>
-      <c r="L54" s="463"/>
-      <c r="M54" s="491" t="s">
+      <c r="L54" s="474"/>
+      <c r="M54" s="480" t="s">
         <v>211</v>
       </c>
-      <c r="N54" s="492"/>
-      <c r="O54" s="492"/>
-      <c r="P54" s="492"/>
-      <c r="Q54" s="493"/>
+      <c r="N54" s="481"/>
+      <c r="O54" s="481"/>
+      <c r="P54" s="481"/>
+      <c r="Q54" s="482"/>
     </row>
     <row r="55" spans="1:17" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D55" s="314" t="s">
@@ -21710,11 +21771,11 @@
       <c r="J55" s="106"/>
       <c r="K55" s="178"/>
       <c r="L55" s="107"/>
-      <c r="M55" s="494"/>
-      <c r="N55" s="495"/>
-      <c r="O55" s="495"/>
-      <c r="P55" s="495"/>
-      <c r="Q55" s="496"/>
+      <c r="M55" s="483"/>
+      <c r="N55" s="484"/>
+      <c r="O55" s="484"/>
+      <c r="P55" s="484"/>
+      <c r="Q55" s="485"/>
     </row>
     <row r="56" spans="1:17" ht="19.5" thickTop="1" x14ac:dyDescent="0.3">
       <c r="C56" s="4" t="s">
@@ -21732,11 +21793,11 @@
         <v>15</v>
       </c>
       <c r="J56" s="109"/>
-      <c r="K56" s="465">
+      <c r="K56" s="476">
         <f>-C4</f>
         <v>-567389.35</v>
       </c>
-      <c r="L56" s="466"/>
+      <c r="L56" s="477"/>
     </row>
     <row r="57" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D57" s="110" t="s">
@@ -21753,22 +21814,22 @@
       <c r="C58" s="112">
         <v>44563</v>
       </c>
-      <c r="D58" s="443" t="s">
+      <c r="D58" s="454" t="s">
         <v>18</v>
       </c>
-      <c r="E58" s="444"/>
+      <c r="E58" s="455"/>
       <c r="F58" s="113">
         <v>754143.23</v>
       </c>
-      <c r="I58" s="445" t="s">
+      <c r="I58" s="456" t="s">
         <v>198</v>
       </c>
-      <c r="J58" s="446"/>
-      <c r="K58" s="447">
+      <c r="J58" s="457"/>
+      <c r="K58" s="458">
         <f>K54+K56</f>
         <v>135803.51000000013</v>
       </c>
-      <c r="L58" s="447"/>
+      <c r="L58" s="458"/>
     </row>
     <row r="59" spans="1:17" ht="17.25" x14ac:dyDescent="0.3">
       <c r="C59" s="114"/>
@@ -21912,13 +21973,20 @@
     </row>
   </sheetData>
   <mergeCells count="30">
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:M1"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="H3:I3"/>
-    <mergeCell ref="P3:P4"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="H4:I4"/>
+    <mergeCell ref="D58:E58"/>
+    <mergeCell ref="I58:J58"/>
+    <mergeCell ref="K58:L58"/>
+    <mergeCell ref="D53:E53"/>
+    <mergeCell ref="D54:E54"/>
+    <mergeCell ref="I54:J54"/>
+    <mergeCell ref="K54:L54"/>
+    <mergeCell ref="M54:Q55"/>
+    <mergeCell ref="K56:L56"/>
+    <mergeCell ref="W27:X28"/>
+    <mergeCell ref="Y27:Y28"/>
+    <mergeCell ref="M36:M37"/>
+    <mergeCell ref="N36:N37"/>
+    <mergeCell ref="Q36:Q37"/>
     <mergeCell ref="H52:I52"/>
     <mergeCell ref="K52:L52"/>
     <mergeCell ref="W4:X5"/>
@@ -21928,20 +21996,13 @@
     <mergeCell ref="W25:X25"/>
     <mergeCell ref="W26:X26"/>
     <mergeCell ref="R3:R4"/>
-    <mergeCell ref="M54:Q55"/>
-    <mergeCell ref="K56:L56"/>
-    <mergeCell ref="W27:X28"/>
-    <mergeCell ref="Y27:Y28"/>
-    <mergeCell ref="M36:M37"/>
-    <mergeCell ref="N36:N37"/>
-    <mergeCell ref="Q36:Q37"/>
-    <mergeCell ref="D58:E58"/>
-    <mergeCell ref="I58:J58"/>
-    <mergeCell ref="K58:L58"/>
-    <mergeCell ref="D53:E53"/>
-    <mergeCell ref="D54:E54"/>
-    <mergeCell ref="I54:J54"/>
-    <mergeCell ref="K54:L54"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:M1"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="P3:P4"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="H4:I4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -24636,7 +24697,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:25" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B1" s="467"/>
+      <c r="B1" s="443"/>
       <c r="C1" s="509" t="s">
         <v>323</v>
       </c>
@@ -24652,7 +24713,7 @@
       <c r="M1" s="510"/>
     </row>
     <row r="2" spans="1:25" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="468"/>
+      <c r="B2" s="444"/>
       <c r="C2" s="3"/>
       <c r="H2" s="5"/>
       <c r="I2" s="6"/>
@@ -24662,21 +24723,21 @@
       <c r="N2" s="9"/>
     </row>
     <row r="3" spans="1:25" ht="21.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="471" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="472"/>
+      <c r="B3" s="447" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="448"/>
       <c r="D3" s="10"/>
       <c r="E3" s="11"/>
       <c r="F3" s="11"/>
-      <c r="H3" s="473" t="s">
+      <c r="H3" s="449" t="s">
         <v>26</v>
       </c>
-      <c r="I3" s="473"/>
+      <c r="I3" s="449"/>
       <c r="K3" s="165"/>
       <c r="L3" s="13"/>
       <c r="M3" s="14"/>
-      <c r="P3" s="497" t="s">
+      <c r="P3" s="486" t="s">
         <v>6</v>
       </c>
       <c r="R3" s="507" t="s">
@@ -24694,14 +24755,14 @@
       <c r="D4" s="18">
         <v>44563</v>
       </c>
-      <c r="E4" s="474" t="s">
+      <c r="E4" s="450" t="s">
         <v>2</v>
       </c>
-      <c r="F4" s="475"/>
-      <c r="H4" s="476" t="s">
+      <c r="F4" s="451"/>
+      <c r="H4" s="452" t="s">
         <v>3</v>
       </c>
-      <c r="I4" s="477"/>
+      <c r="I4" s="453"/>
       <c r="J4" s="19"/>
       <c r="K4" s="166"/>
       <c r="L4" s="20"/>
@@ -24711,15 +24772,15 @@
       <c r="N4" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="P4" s="498"/>
+      <c r="P4" s="487"/>
       <c r="Q4" s="323" t="s">
         <v>217</v>
       </c>
       <c r="R4" s="508"/>
-      <c r="W4" s="480" t="s">
+      <c r="W4" s="496" t="s">
         <v>124</v>
       </c>
-      <c r="X4" s="480"/>
+      <c r="X4" s="496"/>
       <c r="Y4" s="227"/>
     </row>
     <row r="5" spans="1:25" ht="18" thickBot="1" x14ac:dyDescent="0.35">
@@ -24770,8 +24831,8 @@
         <v>0</v>
       </c>
       <c r="S5" s="325"/>
-      <c r="W5" s="480"/>
-      <c r="X5" s="480"/>
+      <c r="W5" s="496"/>
+      <c r="X5" s="496"/>
       <c r="Y5" s="233"/>
     </row>
     <row r="6" spans="1:25" ht="18" thickBot="1" x14ac:dyDescent="0.35">
@@ -25535,7 +25596,7 @@
         <v>0</v>
       </c>
       <c r="S19" s="147"/>
-      <c r="W19" s="484">
+      <c r="W19" s="500">
         <f>SUM(W6:W18)</f>
         <v>0</v>
       </c>
@@ -25588,7 +25649,7 @@
         <v>0</v>
       </c>
       <c r="S20" s="147"/>
-      <c r="W20" s="485"/>
+      <c r="W20" s="501"/>
       <c r="X20" s="268"/>
       <c r="Y20" s="233"/>
     </row>
@@ -25637,8 +25698,8 @@
         <v>377273.87</v>
       </c>
       <c r="S21" s="147"/>
-      <c r="W21" s="486"/>
-      <c r="X21" s="486"/>
+      <c r="W21" s="502"/>
+      <c r="X21" s="502"/>
       <c r="Y21" s="233"/>
       <c r="Z21" s="128"/>
     </row>
@@ -25738,8 +25799,8 @@
         <v>0</v>
       </c>
       <c r="S23" s="147"/>
-      <c r="W23" s="487"/>
-      <c r="X23" s="487"/>
+      <c r="W23" s="503"/>
+      <c r="X23" s="503"/>
       <c r="Y23" s="233"/>
       <c r="Z23" s="128"/>
     </row>
@@ -25794,8 +25855,8 @@
         <v>0</v>
       </c>
       <c r="S24" s="147"/>
-      <c r="W24" s="487"/>
-      <c r="X24" s="487"/>
+      <c r="W24" s="503"/>
+      <c r="X24" s="503"/>
       <c r="Y24" s="233"/>
       <c r="Z24" s="128"/>
     </row>
@@ -25840,8 +25901,8 @@
       <c r="R25" s="320">
         <v>0</v>
       </c>
-      <c r="W25" s="488"/>
-      <c r="X25" s="488"/>
+      <c r="W25" s="504"/>
+      <c r="X25" s="504"/>
       <c r="Y25" s="233"/>
       <c r="Z25" s="128"/>
     </row>
@@ -25889,8 +25950,8 @@
       <c r="R26" s="320">
         <v>0</v>
       </c>
-      <c r="W26" s="488"/>
-      <c r="X26" s="488"/>
+      <c r="W26" s="504"/>
+      <c r="X26" s="504"/>
       <c r="Y26" s="233"/>
       <c r="Z26" s="128"/>
     </row>
@@ -25944,9 +26005,9 @@
       <c r="V27" t="s">
         <v>240</v>
       </c>
-      <c r="W27" s="481"/>
-      <c r="X27" s="482"/>
-      <c r="Y27" s="483"/>
+      <c r="W27" s="497"/>
+      <c r="X27" s="498"/>
+      <c r="Y27" s="499"/>
       <c r="Z27" s="128"/>
     </row>
     <row r="28" spans="1:26" ht="18" thickBot="1" x14ac:dyDescent="0.35">
@@ -26000,9 +26061,9 @@
       <c r="V28" t="s">
         <v>240</v>
       </c>
-      <c r="W28" s="482"/>
-      <c r="X28" s="482"/>
-      <c r="Y28" s="483"/>
+      <c r="W28" s="498"/>
+      <c r="X28" s="498"/>
+      <c r="Y28" s="499"/>
       <c r="Z28" s="128"/>
     </row>
     <row r="29" spans="1:26" ht="18" thickBot="1" x14ac:dyDescent="0.35">
@@ -26307,11 +26368,11 @@
       <c r="L36" s="44">
         <v>13275.84</v>
       </c>
-      <c r="M36" s="499">
+      <c r="M36" s="488">
         <f>SUM(M5:M35)</f>
         <v>1818445.73</v>
       </c>
-      <c r="N36" s="501">
+      <c r="N36" s="490">
         <f>SUM(N5:N35)</f>
         <v>739014</v>
       </c>
@@ -26319,7 +26380,7 @@
       <c r="P36" s="277">
         <v>0</v>
       </c>
-      <c r="Q36" s="503">
+      <c r="Q36" s="492">
         <f>SUM(Q5:Q35)</f>
         <v>-7.2800000000133878</v>
       </c>
@@ -26344,13 +26405,13 @@
       <c r="L37" s="61">
         <v>15060.32</v>
       </c>
-      <c r="M37" s="500"/>
-      <c r="N37" s="502"/>
+      <c r="M37" s="489"/>
+      <c r="N37" s="491"/>
       <c r="O37" s="276"/>
       <c r="P37" s="277">
         <v>0</v>
       </c>
-      <c r="Q37" s="504"/>
+      <c r="Q37" s="493"/>
       <c r="R37" s="227" t="s">
         <v>7</v>
       </c>
@@ -26637,26 +26698,26 @@
       <c r="A52" s="98"/>
       <c r="B52" s="99"/>
       <c r="C52" s="1"/>
-      <c r="H52" s="454" t="s">
+      <c r="H52" s="465" t="s">
         <v>11</v>
       </c>
-      <c r="I52" s="455"/>
+      <c r="I52" s="466"/>
       <c r="J52" s="100"/>
-      <c r="K52" s="456">
+      <c r="K52" s="467">
         <f>I50+L50</f>
         <v>144994.20000000001</v>
       </c>
-      <c r="L52" s="489"/>
+      <c r="L52" s="494"/>
       <c r="M52" s="272"/>
       <c r="N52" s="272"/>
       <c r="P52" s="34"/>
       <c r="Q52" s="13"/>
     </row>
     <row r="53" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="D53" s="460" t="s">
+      <c r="D53" s="471" t="s">
         <v>12</v>
       </c>
-      <c r="E53" s="460"/>
+      <c r="E53" s="471"/>
       <c r="F53" s="313">
         <f>F50-K52-C50</f>
         <v>2135426.1199999996</v>
@@ -26665,22 +26726,22 @@
       <c r="J53" s="103"/>
     </row>
     <row r="54" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="D54" s="490" t="s">
+      <c r="D54" s="495" t="s">
         <v>95</v>
       </c>
-      <c r="E54" s="490"/>
+      <c r="E54" s="495"/>
       <c r="F54" s="111">
         <v>-1448401.2</v>
       </c>
-      <c r="I54" s="461" t="s">
+      <c r="I54" s="472" t="s">
         <v>13</v>
       </c>
-      <c r="J54" s="462"/>
-      <c r="K54" s="463">
+      <c r="J54" s="473"/>
+      <c r="K54" s="474">
         <f>F56+F57+F58</f>
         <v>1082916.0699999996</v>
       </c>
-      <c r="L54" s="463"/>
+      <c r="L54" s="474"/>
       <c r="M54" s="423"/>
       <c r="N54" s="423"/>
       <c r="O54" s="423"/>
@@ -26721,11 +26782,11 @@
         <v>15</v>
       </c>
       <c r="J56" s="109"/>
-      <c r="K56" s="465">
+      <c r="K56" s="476">
         <f>-C4</f>
         <v>-754143.23</v>
       </c>
-      <c r="L56" s="466"/>
+      <c r="L56" s="477"/>
     </row>
     <row r="57" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D57" s="110" t="s">
@@ -26742,22 +26803,22 @@
       <c r="C58" s="112">
         <v>44591</v>
       </c>
-      <c r="D58" s="443" t="s">
+      <c r="D58" s="454" t="s">
         <v>18</v>
       </c>
-      <c r="E58" s="444"/>
+      <c r="E58" s="455"/>
       <c r="F58" s="113">
         <v>1149740.4099999999</v>
       </c>
-      <c r="I58" s="445" t="s">
+      <c r="I58" s="456" t="s">
         <v>198</v>
       </c>
-      <c r="J58" s="446"/>
-      <c r="K58" s="447">
+      <c r="J58" s="457"/>
+      <c r="K58" s="458">
         <f>K54+K56</f>
         <v>328772.83999999962</v>
       </c>
-      <c r="L58" s="447"/>
+      <c r="L58" s="458"/>
     </row>
     <row r="59" spans="1:17" ht="17.25" x14ac:dyDescent="0.3">
       <c r="C59" s="114"/>
@@ -26901,6 +26962,20 @@
     </row>
   </sheetData>
   <mergeCells count="29">
+    <mergeCell ref="Y27:Y28"/>
+    <mergeCell ref="M36:M37"/>
+    <mergeCell ref="N36:N37"/>
+    <mergeCell ref="Q36:Q37"/>
+    <mergeCell ref="D58:E58"/>
+    <mergeCell ref="I58:J58"/>
+    <mergeCell ref="K58:L58"/>
+    <mergeCell ref="D53:E53"/>
+    <mergeCell ref="D54:E54"/>
+    <mergeCell ref="I54:J54"/>
+    <mergeCell ref="K54:L54"/>
+    <mergeCell ref="K56:L56"/>
+    <mergeCell ref="H52:I52"/>
+    <mergeCell ref="K52:L52"/>
     <mergeCell ref="W26:X26"/>
     <mergeCell ref="R3:R4"/>
     <mergeCell ref="W27:X28"/>
@@ -26916,20 +26991,6 @@
     <mergeCell ref="W21:X21"/>
     <mergeCell ref="W23:X24"/>
     <mergeCell ref="W25:X25"/>
-    <mergeCell ref="Y27:Y28"/>
-    <mergeCell ref="M36:M37"/>
-    <mergeCell ref="N36:N37"/>
-    <mergeCell ref="Q36:Q37"/>
-    <mergeCell ref="D58:E58"/>
-    <mergeCell ref="I58:J58"/>
-    <mergeCell ref="K58:L58"/>
-    <mergeCell ref="D53:E53"/>
-    <mergeCell ref="D54:E54"/>
-    <mergeCell ref="I54:J54"/>
-    <mergeCell ref="K54:L54"/>
-    <mergeCell ref="K56:L56"/>
-    <mergeCell ref="H52:I52"/>
-    <mergeCell ref="K52:L52"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -29684,8 +29745,8 @@
   </sheetPr>
   <dimension ref="A1:Z80"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G19" workbookViewId="0">
-      <selection activeCell="M28" sqref="M28"/>
+    <sheetView tabSelected="1" topLeftCell="B37" workbookViewId="0">
+      <selection activeCell="F59" sqref="F59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -29714,7 +29775,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:25" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B1" s="467"/>
+      <c r="B1" s="443"/>
       <c r="C1" s="509" t="s">
         <v>323</v>
       </c>
@@ -29730,7 +29791,7 @@
       <c r="M1" s="510"/>
     </row>
     <row r="2" spans="1:25" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="468"/>
+      <c r="B2" s="444"/>
       <c r="C2" s="3"/>
       <c r="H2" s="5"/>
       <c r="I2" s="6"/>
@@ -29740,21 +29801,21 @@
       <c r="N2" s="9"/>
     </row>
     <row r="3" spans="1:25" ht="21.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="471" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="472"/>
+      <c r="B3" s="447" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="448"/>
       <c r="D3" s="10"/>
       <c r="E3" s="11"/>
       <c r="F3" s="11"/>
-      <c r="H3" s="473" t="s">
+      <c r="H3" s="449" t="s">
         <v>26</v>
       </c>
-      <c r="I3" s="473"/>
+      <c r="I3" s="449"/>
       <c r="K3" s="165"/>
       <c r="L3" s="13"/>
       <c r="M3" s="14"/>
-      <c r="P3" s="497" t="s">
+      <c r="P3" s="486" t="s">
         <v>6</v>
       </c>
       <c r="R3" s="507" t="s">
@@ -29772,14 +29833,14 @@
       <c r="D4" s="18">
         <v>44591</v>
       </c>
-      <c r="E4" s="474" t="s">
+      <c r="E4" s="450" t="s">
         <v>2</v>
       </c>
-      <c r="F4" s="475"/>
-      <c r="H4" s="476" t="s">
+      <c r="F4" s="451"/>
+      <c r="H4" s="452" t="s">
         <v>3</v>
       </c>
-      <c r="I4" s="477"/>
+      <c r="I4" s="453"/>
       <c r="J4" s="19"/>
       <c r="K4" s="166"/>
       <c r="L4" s="20"/>
@@ -29789,15 +29850,15 @@
       <c r="N4" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="P4" s="498"/>
+      <c r="P4" s="487"/>
       <c r="Q4" s="323" t="s">
         <v>217</v>
       </c>
       <c r="R4" s="508"/>
-      <c r="W4" s="480" t="s">
+      <c r="W4" s="496" t="s">
         <v>124</v>
       </c>
-      <c r="X4" s="480"/>
+      <c r="X4" s="496"/>
       <c r="Y4" s="227"/>
     </row>
     <row r="5" spans="1:25" ht="18" thickBot="1" x14ac:dyDescent="0.35">
@@ -29848,8 +29909,8 @@
         <v>0</v>
       </c>
       <c r="S5" s="325"/>
-      <c r="W5" s="480"/>
-      <c r="X5" s="480"/>
+      <c r="W5" s="496"/>
+      <c r="X5" s="496"/>
       <c r="Y5" s="233"/>
     </row>
     <row r="6" spans="1:25" ht="18" thickBot="1" x14ac:dyDescent="0.35">
@@ -30610,7 +30671,7 @@
         <v>0</v>
       </c>
       <c r="S19" s="147"/>
-      <c r="W19" s="484">
+      <c r="W19" s="500">
         <f>SUM(W6:W18)</f>
         <v>0</v>
       </c>
@@ -30654,7 +30715,7 @@
         <f t="shared" si="0"/>
         <v>72030</v>
       </c>
-      <c r="Q20" s="318">
+      <c r="Q20" s="326">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -30662,7 +30723,7 @@
         <v>0</v>
       </c>
       <c r="S20" s="147"/>
-      <c r="W20" s="485"/>
+      <c r="W20" s="501"/>
       <c r="X20" s="268"/>
       <c r="Y20" s="233"/>
     </row>
@@ -30711,8 +30772,8 @@
         <v>18072</v>
       </c>
       <c r="S21" s="147"/>
-      <c r="W21" s="486"/>
-      <c r="X21" s="486"/>
+      <c r="W21" s="502"/>
+      <c r="X21" s="502"/>
       <c r="Y21" s="233"/>
       <c r="Z21" s="128"/>
     </row>
@@ -30753,7 +30814,7 @@
         <f t="shared" si="0"/>
         <v>78137</v>
       </c>
-      <c r="Q22" s="318">
+      <c r="Q22" s="326">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -30803,7 +30864,7 @@
         <f t="shared" si="0"/>
         <v>103716</v>
       </c>
-      <c r="Q23" s="318">
+      <c r="Q23" s="326">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -30811,8 +30872,8 @@
         <v>0</v>
       </c>
       <c r="S23" s="147"/>
-      <c r="W23" s="487"/>
-      <c r="X23" s="487"/>
+      <c r="W23" s="503"/>
+      <c r="X23" s="503"/>
       <c r="Y23" s="233"/>
       <c r="Z23" s="128"/>
     </row>
@@ -30859,7 +30920,7 @@
         <f>N24+M24+L24+I24+C24</f>
         <v>167635</v>
       </c>
-      <c r="Q24" s="318">
+      <c r="Q24" s="326">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -30867,8 +30928,8 @@
         <v>0</v>
       </c>
       <c r="S24" s="147"/>
-      <c r="W24" s="487"/>
-      <c r="X24" s="487"/>
+      <c r="W24" s="503"/>
+      <c r="X24" s="503"/>
       <c r="Y24" s="233"/>
       <c r="Z24" s="128"/>
     </row>
@@ -30909,15 +30970,15 @@
         <f t="shared" si="0"/>
         <v>78995.5</v>
       </c>
-      <c r="Q25" s="318">
+      <c r="Q25" s="326">
         <f t="shared" si="1"/>
         <v>4.5</v>
       </c>
       <c r="R25" s="320">
         <v>0</v>
       </c>
-      <c r="W25" s="488"/>
-      <c r="X25" s="488"/>
+      <c r="W25" s="504"/>
+      <c r="X25" s="504"/>
       <c r="Y25" s="233"/>
       <c r="Z25" s="128"/>
     </row>
@@ -30958,15 +31019,15 @@
         <f t="shared" si="0"/>
         <v>97381</v>
       </c>
-      <c r="Q26" s="318">
+      <c r="Q26" s="326">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="R26" s="320">
         <v>0</v>
       </c>
-      <c r="W26" s="488"/>
-      <c r="X26" s="488"/>
+      <c r="W26" s="504"/>
+      <c r="X26" s="504"/>
       <c r="Y26" s="233"/>
       <c r="Z26" s="128"/>
     </row>
@@ -31007,16 +31068,16 @@
         <f t="shared" si="0"/>
         <v>55967.4</v>
       </c>
-      <c r="Q27" s="318">
+      <c r="Q27" s="326">
         <f t="shared" si="1"/>
         <v>0.40000000000145519</v>
       </c>
       <c r="R27" s="320">
         <v>0</v>
       </c>
-      <c r="W27" s="481"/>
-      <c r="X27" s="482"/>
-      <c r="Y27" s="483"/>
+      <c r="W27" s="497"/>
+      <c r="X27" s="498"/>
+      <c r="Y27" s="499"/>
       <c r="Z27" s="128"/>
     </row>
     <row r="28" spans="1:26" ht="18" thickBot="1" x14ac:dyDescent="0.35">
@@ -31057,16 +31118,16 @@
         <f t="shared" si="0"/>
         <v>75249</v>
       </c>
-      <c r="Q28" s="318">
+      <c r="Q28" s="326">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="R28" s="320">
         <v>0</v>
       </c>
-      <c r="W28" s="482"/>
-      <c r="X28" s="482"/>
-      <c r="Y28" s="483"/>
+      <c r="W28" s="498"/>
+      <c r="X28" s="498"/>
+      <c r="Y28" s="499"/>
       <c r="Z28" s="128"/>
     </row>
     <row r="29" spans="1:26" ht="18" thickBot="1" x14ac:dyDescent="0.35">
@@ -31075,41 +31136,51 @@
         <v>44616</v>
       </c>
       <c r="C29" s="25">
-        <v>0</v>
-      </c>
-      <c r="D29" s="58"/>
+        <v>6774</v>
+      </c>
+      <c r="D29" s="58" t="s">
+        <v>452</v>
+      </c>
       <c r="E29" s="27">
         <v>44616</v>
       </c>
       <c r="F29" s="28">
-        <v>0</v>
+        <v>65978</v>
       </c>
       <c r="G29" s="2"/>
       <c r="H29" s="36">
         <v>44616</v>
       </c>
       <c r="I29" s="30">
-        <v>0</v>
+        <v>1660</v>
       </c>
       <c r="J29" s="59"/>
       <c r="K29" s="175"/>
       <c r="L29" s="54"/>
       <c r="M29" s="32">
-        <v>0</v>
-      </c>
-      <c r="N29" s="33">
-        <v>0</v>
+        <f>3507.28+46135</f>
+        <v>49642.28</v>
+      </c>
+      <c r="N29" s="548">
+        <f>7491+411</f>
+        <v>7902</v>
+      </c>
+      <c r="O29" s="551" t="s">
+        <v>455</v>
       </c>
       <c r="P29" s="34">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="Q29" s="318">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <v>65978.28</v>
+      </c>
+      <c r="Q29" s="326">
+        <f t="shared" si="1"/>
+        <v>0.27999999999883585</v>
       </c>
       <c r="R29" s="320">
         <v>0</v>
+      </c>
+      <c r="T29" s="553">
+        <v>7491</v>
       </c>
       <c r="U29" s="337"/>
       <c r="W29" s="128"/>
@@ -31123,40 +31194,50 @@
         <v>44617</v>
       </c>
       <c r="C30" s="25">
-        <v>0</v>
-      </c>
-      <c r="D30" s="58"/>
+        <v>10378</v>
+      </c>
+      <c r="D30" s="58" t="s">
+        <v>454</v>
+      </c>
       <c r="E30" s="27">
         <v>44617</v>
       </c>
       <c r="F30" s="28">
-        <v>0</v>
+        <v>749838</v>
       </c>
       <c r="G30" s="2"/>
       <c r="H30" s="36">
         <v>44617</v>
       </c>
       <c r="I30" s="30">
-        <v>0</v>
+        <v>1490</v>
       </c>
       <c r="J30" s="60"/>
       <c r="K30" s="41"/>
       <c r="L30" s="61"/>
       <c r="M30" s="32">
-        <v>0</v>
-      </c>
-      <c r="N30" s="33">
-        <v>0</v>
+        <f>680259.73+69394+54204.48</f>
+        <v>803858.21</v>
+      </c>
+      <c r="N30" s="548">
+        <v>26626</v>
+      </c>
+      <c r="O30" s="552" t="s">
+        <v>453</v>
       </c>
       <c r="P30" s="34">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="Q30" s="318">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="R30" s="321"/>
+        <v>842352.21</v>
+      </c>
+      <c r="Q30" s="326">
+        <v>0</v>
+      </c>
+      <c r="R30" s="550">
+        <v>92514</v>
+      </c>
+      <c r="T30" s="553">
+        <v>26626</v>
+      </c>
       <c r="X30" s="225"/>
       <c r="Y30" s="227"/>
     </row>
@@ -31166,40 +31247,58 @@
         <v>44618</v>
       </c>
       <c r="C31" s="25">
-        <v>0</v>
-      </c>
-      <c r="D31" s="65"/>
+        <v>6319</v>
+      </c>
+      <c r="D31" s="65" t="s">
+        <v>456</v>
+      </c>
       <c r="E31" s="27">
         <v>44618</v>
       </c>
       <c r="F31" s="28">
-        <v>0</v>
+        <v>107356</v>
       </c>
       <c r="G31" s="2"/>
       <c r="H31" s="36">
         <v>44618</v>
       </c>
       <c r="I31" s="30">
-        <v>0</v>
-      </c>
-      <c r="J31" s="60"/>
-      <c r="K31" s="41"/>
-      <c r="L31" s="63"/>
+        <v>4829</v>
+      </c>
+      <c r="J31" s="60">
+        <v>44618</v>
+      </c>
+      <c r="K31" s="41" t="s">
+        <v>457</v>
+      </c>
+      <c r="L31" s="63">
+        <v>16621.14</v>
+      </c>
       <c r="M31" s="32">
-        <v>0</v>
-      </c>
-      <c r="N31" s="33">
-        <v>0</v>
+        <f>998+41741</f>
+        <v>42739</v>
+      </c>
+      <c r="N31" s="548">
+        <f>10137+26711</f>
+        <v>36848</v>
+      </c>
+      <c r="O31" s="551" t="s">
+        <v>455</v>
       </c>
       <c r="P31" s="34">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="Q31" s="287">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="R31" s="322"/>
+        <v>107356.14</v>
+      </c>
+      <c r="Q31" s="111">
+        <f t="shared" si="1"/>
+        <v>0.13999999999941792</v>
+      </c>
+      <c r="R31" s="322">
+        <v>0</v>
+      </c>
+      <c r="T31" s="553">
+        <v>10137</v>
+      </c>
     </row>
     <row r="32" spans="1:26" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A32" s="23"/>
@@ -31207,44 +31306,50 @@
         <v>44619</v>
       </c>
       <c r="C32" s="25">
-        <v>0</v>
-      </c>
-      <c r="D32" s="64"/>
+        <v>3900</v>
+      </c>
+      <c r="D32" s="64" t="s">
+        <v>459</v>
+      </c>
       <c r="E32" s="27">
         <v>44619</v>
       </c>
       <c r="F32" s="28">
-        <v>0</v>
+        <v>86103</v>
       </c>
       <c r="G32" s="2"/>
       <c r="H32" s="36">
         <v>44619</v>
       </c>
       <c r="I32" s="30">
-        <v>0</v>
+        <v>1109</v>
       </c>
       <c r="J32" s="60"/>
       <c r="K32" s="41"/>
       <c r="L32" s="61"/>
       <c r="M32" s="32">
-        <v>0</v>
+        <f>51650+7128</f>
+        <v>58778</v>
       </c>
       <c r="N32" s="33">
-        <v>0</v>
+        <v>22320</v>
       </c>
       <c r="P32" s="34">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="Q32" s="287">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <v>86107</v>
+      </c>
+      <c r="Q32" s="111">
+        <f t="shared" si="1"/>
+        <v>4</v>
       </c>
       <c r="R32" s="228">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="33" spans="1:18" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+        <v>0</v>
+      </c>
+      <c r="T32" s="553">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:20" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A33" s="23"/>
       <c r="B33" s="24"/>
       <c r="C33" s="25"/>
@@ -31266,13 +31371,17 @@
       <c r="P33" s="34">
         <v>0</v>
       </c>
-      <c r="Q33" s="287">
+      <c r="Q33" s="111">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="R33" s="228"/>
-    </row>
-    <row r="34" spans="1:18" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="T33" s="554">
+        <f>SUM(T29:T32)</f>
+        <v>44254</v>
+      </c>
+    </row>
+    <row r="34" spans="1:20" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A34" s="23"/>
       <c r="B34" s="24"/>
       <c r="C34" s="25"/>
@@ -31294,13 +31403,13 @@
       <c r="P34" s="34">
         <v>0</v>
       </c>
-      <c r="Q34" s="287">
+      <c r="Q34" s="111">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="R34" s="228"/>
     </row>
-    <row r="35" spans="1:18" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:20" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A35" s="23"/>
       <c r="B35" s="24"/>
       <c r="C35" s="25"/>
@@ -31322,13 +31431,13 @@
       <c r="P35" s="34">
         <v>0</v>
       </c>
-      <c r="Q35" s="273">
+      <c r="Q35" s="549">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="R35" s="228"/>
     </row>
-    <row r="36" spans="1:18" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:20" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="23"/>
       <c r="B36" s="24"/>
       <c r="C36" s="25"/>
@@ -31341,25 +31450,25 @@
       <c r="J36" s="266"/>
       <c r="K36" s="250"/>
       <c r="L36" s="44"/>
-      <c r="M36" s="499">
+      <c r="M36" s="488">
         <f>SUM(M5:M35)</f>
-        <v>1188847</v>
-      </c>
-      <c r="N36" s="501">
+        <v>2143864.4900000002</v>
+      </c>
+      <c r="N36" s="490">
         <f>SUM(N5:N35)</f>
-        <v>697412</v>
+        <v>791108</v>
       </c>
       <c r="O36" s="276"/>
       <c r="P36" s="277">
         <v>0</v>
       </c>
-      <c r="Q36" s="503">
+      <c r="Q36" s="555">
         <f>SUM(Q5:Q35)</f>
-        <v>107.0199999999968</v>
+        <v>111.43999999999505</v>
       </c>
       <c r="R36" s="228"/>
     </row>
-    <row r="37" spans="1:18" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:20" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="23"/>
       <c r="B37" s="24"/>
       <c r="C37" s="25"/>
@@ -31378,18 +31487,18 @@
       <c r="L37" s="61">
         <v>16518.78</v>
       </c>
-      <c r="M37" s="500"/>
-      <c r="N37" s="502"/>
+      <c r="M37" s="489"/>
+      <c r="N37" s="491"/>
       <c r="O37" s="276"/>
       <c r="P37" s="277">
         <v>0</v>
       </c>
-      <c r="Q37" s="504"/>
+      <c r="Q37" s="556"/>
       <c r="R37" s="227" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="38" spans="1:18" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:20" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A38" s="23"/>
       <c r="B38" s="24"/>
       <c r="C38" s="25"/>
@@ -31415,7 +31524,7 @@
       </c>
       <c r="Q38" s="274"/>
     </row>
-    <row r="39" spans="1:18" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:20" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A39" s="23"/>
       <c r="B39" s="24"/>
       <c r="C39" s="69"/>
@@ -31434,15 +31543,18 @@
       <c r="L39" s="61">
         <v>14981.03</v>
       </c>
-      <c r="M39" s="278"/>
-      <c r="N39" s="278"/>
+      <c r="M39" s="557">
+        <f>M36+N36</f>
+        <v>2934972.49</v>
+      </c>
+      <c r="N39" s="558"/>
       <c r="P39" s="34">
         <f>SUM(P5:P38)</f>
-        <v>2348286.02</v>
+        <v>3450079.65</v>
       </c>
       <c r="Q39" s="275"/>
     </row>
-    <row r="40" spans="1:18" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:20" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A40" s="23"/>
       <c r="B40" s="24"/>
       <c r="C40" s="69"/>
@@ -31452,15 +31564,21 @@
       <c r="G40" s="2"/>
       <c r="H40" s="36"/>
       <c r="I40" s="71"/>
-      <c r="J40" s="60"/>
-      <c r="K40" s="41"/>
-      <c r="L40" s="61"/>
+      <c r="J40" s="60" t="s">
+        <v>429</v>
+      </c>
+      <c r="K40" s="41" t="s">
+        <v>458</v>
+      </c>
+      <c r="L40" s="61">
+        <v>13372.77</v>
+      </c>
       <c r="M40" s="278"/>
       <c r="N40" s="278"/>
       <c r="P40" s="34"/>
       <c r="Q40" s="13"/>
     </row>
-    <row r="41" spans="1:18" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:20" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A41" s="23"/>
       <c r="B41" s="24"/>
       <c r="C41" s="72"/>
@@ -31478,7 +31596,7 @@
       <c r="P41" s="34"/>
       <c r="Q41" s="13"/>
     </row>
-    <row r="42" spans="1:18" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:20" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A42" s="23"/>
       <c r="B42" s="24"/>
       <c r="C42" s="72"/>
@@ -31496,7 +31614,7 @@
       <c r="P42" s="34"/>
       <c r="Q42" s="13"/>
     </row>
-    <row r="43" spans="1:18" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:20" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A43" s="23"/>
       <c r="B43" s="24"/>
       <c r="C43" s="72"/>
@@ -31514,7 +31632,7 @@
       <c r="P43" s="34"/>
       <c r="Q43" s="13"/>
     </row>
-    <row r="44" spans="1:18" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:20" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A44" s="23"/>
       <c r="B44" s="24"/>
       <c r="C44" s="72"/>
@@ -31532,7 +31650,7 @@
       <c r="P44" s="34"/>
       <c r="Q44" s="13"/>
     </row>
-    <row r="45" spans="1:18" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:20" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A45" s="23"/>
       <c r="B45" s="24"/>
       <c r="C45" s="72"/>
@@ -31550,7 +31668,7 @@
       <c r="P45" s="34"/>
       <c r="Q45" s="13"/>
     </row>
-    <row r="46" spans="1:18" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:20" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A46" s="23"/>
       <c r="B46" s="24"/>
       <c r="C46" s="72"/>
@@ -31568,7 +31686,7 @@
       <c r="P46" s="34"/>
       <c r="Q46" s="13"/>
     </row>
-    <row r="47" spans="1:18" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:20" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A47" s="23"/>
       <c r="B47" s="24"/>
       <c r="C47" s="72"/>
@@ -31586,7 +31704,7 @@
       <c r="P47" s="34"/>
       <c r="Q47" s="13"/>
     </row>
-    <row r="48" spans="1:18" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:20" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A48" s="23"/>
       <c r="B48" s="24"/>
       <c r="C48" s="72"/>
@@ -31629,7 +31747,7 @@
       </c>
       <c r="C50" s="87">
         <f>SUM(C5:C49)</f>
-        <v>370034.9</v>
+        <v>397405.9</v>
       </c>
       <c r="D50" s="88"/>
       <c r="E50" s="89" t="s">
@@ -31637,7 +31755,7 @@
       </c>
       <c r="F50" s="90">
         <f>SUM(F5:F49)</f>
-        <v>2285541</v>
+        <v>3294816</v>
       </c>
       <c r="G50" s="88"/>
       <c r="H50" s="91" t="s">
@@ -31645,7 +31763,7 @@
       </c>
       <c r="I50" s="92">
         <f>SUM(I5:I49)</f>
-        <v>56595</v>
+        <v>65683</v>
       </c>
       <c r="J50" s="93"/>
       <c r="K50" s="94" t="s">
@@ -31653,7 +31771,7 @@
       </c>
       <c r="L50" s="95">
         <f>SUM(L5:L49)</f>
-        <v>84515.709999999992</v>
+        <v>114509.62</v>
       </c>
       <c r="M50" s="96"/>
       <c r="N50" s="96"/>
@@ -31671,50 +31789,50 @@
       <c r="A52" s="98"/>
       <c r="B52" s="99"/>
       <c r="C52" s="1"/>
-      <c r="H52" s="454" t="s">
+      <c r="H52" s="465" t="s">
         <v>11</v>
       </c>
-      <c r="I52" s="455"/>
+      <c r="I52" s="466"/>
       <c r="J52" s="100"/>
-      <c r="K52" s="456">
+      <c r="K52" s="467">
         <f>I50+L50</f>
-        <v>141110.71</v>
-      </c>
-      <c r="L52" s="489"/>
+        <v>180192.62</v>
+      </c>
+      <c r="L52" s="494"/>
       <c r="M52" s="272"/>
       <c r="N52" s="272"/>
       <c r="P52" s="34"/>
       <c r="Q52" s="13"/>
     </row>
     <row r="53" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="D53" s="460" t="s">
+      <c r="D53" s="471" t="s">
         <v>12</v>
       </c>
-      <c r="E53" s="460"/>
+      <c r="E53" s="471"/>
       <c r="F53" s="313">
         <f>F50-K52-C50</f>
-        <v>1774395.3900000001</v>
+        <v>2717217.48</v>
       </c>
       <c r="I53" s="102"/>
       <c r="J53" s="103"/>
     </row>
     <row r="54" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="D54" s="490" t="s">
+      <c r="D54" s="495" t="s">
         <v>95</v>
       </c>
-      <c r="E54" s="490"/>
+      <c r="E54" s="495"/>
       <c r="F54" s="111">
         <v>0</v>
       </c>
-      <c r="I54" s="461" t="s">
+      <c r="I54" s="472" t="s">
         <v>13</v>
       </c>
-      <c r="J54" s="462"/>
-      <c r="K54" s="463">
+      <c r="J54" s="473"/>
+      <c r="K54" s="474">
         <f>F56+F57+F58</f>
-        <v>1774395.3900000001</v>
-      </c>
-      <c r="L54" s="463"/>
+        <v>3983785.9299999997</v>
+      </c>
+      <c r="L54" s="474"/>
       <c r="M54" s="423"/>
       <c r="N54" s="423"/>
       <c r="O54" s="423"/>
@@ -31748,18 +31866,18 @@
       </c>
       <c r="F56" s="96">
         <f>SUM(F53:F55)</f>
-        <v>1774395.3900000001</v>
+        <v>2717217.48</v>
       </c>
       <c r="H56" s="23"/>
       <c r="I56" s="108" t="s">
         <v>15</v>
       </c>
       <c r="J56" s="109"/>
-      <c r="K56" s="465">
+      <c r="K56" s="476">
         <f>-C4</f>
         <v>-1149740.4099999999</v>
       </c>
-      <c r="L56" s="466"/>
+      <c r="L56" s="477"/>
     </row>
     <row r="57" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D57" s="110" t="s">
@@ -31773,23 +31891,25 @@
       </c>
     </row>
     <row r="58" spans="1:17" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C58" s="112"/>
-      <c r="D58" s="443" t="s">
+      <c r="C58" s="112">
+        <v>44619</v>
+      </c>
+      <c r="D58" s="454" t="s">
         <v>18</v>
       </c>
-      <c r="E58" s="444"/>
+      <c r="E58" s="455"/>
       <c r="F58" s="113">
-        <v>0</v>
-      </c>
-      <c r="I58" s="445" t="s">
+        <v>1266568.45</v>
+      </c>
+      <c r="I58" s="456" t="s">
         <v>198</v>
       </c>
-      <c r="J58" s="446"/>
-      <c r="K58" s="447">
+      <c r="J58" s="457"/>
+      <c r="K58" s="458">
         <f>K54+K56</f>
-        <v>624654.98000000021</v>
-      </c>
-      <c r="L58" s="447"/>
+        <v>2834045.5199999996</v>
+      </c>
+      <c r="L58" s="458"/>
     </row>
     <row r="59" spans="1:17" ht="17.25" x14ac:dyDescent="0.3">
       <c r="C59" s="114"/>
@@ -31932,21 +32052,7 @@
       <c r="F80" s="129"/>
     </row>
   </sheetData>
-  <mergeCells count="29">
-    <mergeCell ref="W26:X26"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:M1"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="H3:I3"/>
-    <mergeCell ref="P3:P4"/>
-    <mergeCell ref="R3:R4"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="H4:I4"/>
-    <mergeCell ref="W4:X5"/>
-    <mergeCell ref="W19:W20"/>
-    <mergeCell ref="W21:X21"/>
-    <mergeCell ref="W23:X24"/>
-    <mergeCell ref="W25:X25"/>
+  <mergeCells count="30">
     <mergeCell ref="D58:E58"/>
     <mergeCell ref="I58:J58"/>
     <mergeCell ref="K58:L58"/>
@@ -31962,6 +32068,21 @@
     <mergeCell ref="I54:J54"/>
     <mergeCell ref="K54:L54"/>
     <mergeCell ref="K56:L56"/>
+    <mergeCell ref="M39:N39"/>
+    <mergeCell ref="W26:X26"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:M1"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="P3:P4"/>
+    <mergeCell ref="R3:R4"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="H4:I4"/>
+    <mergeCell ref="W4:X5"/>
+    <mergeCell ref="W19:W20"/>
+    <mergeCell ref="W21:X21"/>
+    <mergeCell ref="W23:X24"/>
+    <mergeCell ref="W25:X25"/>
   </mergeCells>
   <pageMargins left="0.23" right="0.23" top="0.4" bottom="0.28000000000000003" header="0.3" footer="0.3"/>
   <pageSetup orientation="landscape" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>